<commit_message>
started better integration with core classes
</commit_message>
<xml_diff>
--- a/data/TR/results/PVRP_All_Long_Solutions.xlsx
+++ b/data/TR/results/PVRP_All_Long_Solutions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2430" uniqueCount="30">
   <si>
     <t>Filename</t>
   </si>
@@ -111,13 +111,133 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="31">
+  <fonts count="55">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -310,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
@@ -412,6 +532,86 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -16615,16 +16815,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.11328125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="84.01171875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.2890625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.90625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.7734375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.5078125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.484375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="84.26171875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.39453125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.9140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.796875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.9765625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="58">
+      <c r="A1" t="s" s="106">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -16632,7 +16832,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="57">
+      <c r="A2" t="s" s="105">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -16640,7 +16840,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="57">
+      <c r="A3" t="s" s="105">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -16648,7 +16848,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="57">
+      <c r="A4" t="s" s="105">
         <v>6</v>
       </c>
       <c r="B4" t="n">
@@ -16656,15 +16856,15 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="57">
+      <c r="A5" t="s" s="105">
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>1972.1025390625</v>
+        <v>2019.185791015625</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="57">
+      <c r="A6" t="s" s="105">
         <v>8</v>
       </c>
       <c r="B6" t="n">
@@ -16672,11 +16872,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="57">
+      <c r="A7" t="s" s="105">
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>1.972102665580078E10</v>
+        <v>2.0191859480507812E10</v>
       </c>
     </row>
     <row r="8"/>
@@ -16684,71 +16884,71 @@
     <row r="10"/>
     <row r="11"/>
     <row r="12">
-      <c r="A12" t="s" s="55">
+      <c r="A12" t="s" s="103">
         <v>10</v>
       </c>
-      <c r="B12" t="n" s="56">
+      <c r="B12" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="C12" t="s" s="55">
+      <c r="C12" t="s" s="103">
         <v>11</v>
       </c>
-      <c r="D12" t="n" s="56">
+      <c r="D12" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="E12" t="s" s="55">
+      <c r="E12" t="s" s="103">
         <v>12</v>
       </c>
-      <c r="F12" t="n" s="56">
+      <c r="F12" t="n" s="104">
         <v>-1.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="55">
+      <c r="A13" t="s" s="103">
         <v>13</v>
       </c>
-      <c r="B13" t="n" s="56">
+      <c r="B13" t="n" s="104">
         <v>0.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="55">
+      <c r="A14" t="s" s="103">
         <v>14</v>
       </c>
-      <c r="B14" t="n" s="56">
+      <c r="B14" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="C14" t="s" s="55">
+      <c r="C14" t="s" s="103">
         <v>15</v>
       </c>
-      <c r="D14" t="n" s="56">
+      <c r="D14" t="n" s="104">
         <v>160.0</v>
       </c>
-      <c r="E14" t="s" s="55">
+      <c r="E14" t="s" s="103">
         <v>16</v>
       </c>
-      <c r="F14" t="n" s="60">
-        <v>520.0</v>
+      <c r="F14" t="n" s="108">
+        <v>540.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s" s="55">
+      <c r="A15" t="s" s="103">
         <v>17</v>
       </c>
-      <c r="B15" t="n" s="56">
-        <v>3.0180735852929688E9</v>
-      </c>
-      <c r="C15" t="s" s="55">
+      <c r="B15" t="n" s="104">
+        <v>3.6276982190820312E9</v>
+      </c>
+      <c r="C15" t="s" s="103">
         <v>18</v>
       </c>
-      <c r="D15" t="n" s="56">
+      <c r="D15" t="n" s="104">
         <v>9999999.0</v>
       </c>
-      <c r="E15" t="s" s="55">
+      <c r="E15" t="s" s="103">
         <v>19</v>
       </c>
-      <c r="F15" t="n" s="59">
-        <v>301.8073425292969</v>
+      <c r="F15" t="n" s="107">
+        <v>362.7698059082031</v>
       </c>
     </row>
     <row r="16"/>
@@ -16794,19 +16994,19 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>40.0</v>
+        <v>13.0</v>
       </c>
       <c r="B19" t="n">
-        <v>7.0</v>
+        <v>23.0</v>
       </c>
       <c r="C19" t="n">
-        <v>42.20189666748047</v>
+        <v>29.154760360717773</v>
       </c>
       <c r="D19" t="n">
         <v>8.319952741629265</v>
       </c>
       <c r="E19" t="n">
-        <v>7.8102498054504395</v>
+        <v>25.495098114013672</v>
       </c>
       <c r="F19" t="n">
         <v>1.0</v>
@@ -16814,19 +17014,19 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>41.0</v>
+        <v>25.0</v>
       </c>
       <c r="B20" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="C20" t="n">
-        <v>30.479501724243164</v>
+        <v>23.0867919921875</v>
       </c>
       <c r="D20" t="n">
-        <v>298.9856443268601</v>
+        <v>240.25810175410237</v>
       </c>
       <c r="E20" t="n">
-        <v>12.083045959472656</v>
+        <v>13.152946472167969</v>
       </c>
       <c r="F20" t="n">
         <v>1.0</v>
@@ -16834,19 +17034,19 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>4.0</v>
+        <v>14.0</v>
       </c>
       <c r="B21" t="n">
-        <v>9.0</v>
+        <v>21.0</v>
       </c>
       <c r="C21" t="n">
-        <v>17.20465087890625</v>
+        <v>18.11077117919922</v>
       </c>
       <c r="D21" t="n">
-        <v>206.94372235198546</v>
+        <v>346.6473834054614</v>
       </c>
       <c r="E21" t="n">
-        <v>13.45362377166748</v>
+        <v>6.4031243324279785</v>
       </c>
       <c r="F21" t="n">
         <v>1.0</v>
@@ -16854,19 +17054,19 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>51.0</v>
+        <v>24.0</v>
       </c>
       <c r="B22" t="n">
-        <v>160.0</v>
+        <v>10.0</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0</v>
+        <v>25.05992889404297</v>
       </c>
       <c r="D22" t="n">
-        <v>6.338943043987854</v>
+        <v>171.97940109631875</v>
       </c>
       <c r="E22" t="n">
-        <v>17.20465087890625</v>
+        <v>10.770329475402832</v>
       </c>
       <c r="F22" t="n">
         <v>1.0</v>
@@ -16874,19 +17074,19 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>46.0</v>
+        <v>43.0</v>
       </c>
       <c r="B23" t="n">
-        <v>5.0</v>
+        <v>11.0</v>
       </c>
       <c r="C23" t="n">
-        <v>2.2360680103302</v>
+        <v>34.65544509887695</v>
       </c>
       <c r="D23" t="n">
-        <v>251.4270412434094</v>
+        <v>8.319952741629265</v>
       </c>
       <c r="E23" t="n">
-        <v>2.2360680103302</v>
+        <v>12.369317054748535</v>
       </c>
       <c r="F23" t="n">
         <v>1.0</v>
@@ -16894,19 +17094,19 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>32.0</v>
+        <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>12.0</v>
+        <v>16.0</v>
       </c>
       <c r="C24" t="n">
-        <v>10.0</v>
+        <v>22.022714614868164</v>
       </c>
       <c r="D24" t="n">
-        <v>276.470003989416</v>
+        <v>299.7015117237478</v>
       </c>
       <c r="E24" t="n">
-        <v>9.219544410705566</v>
+        <v>13.03840446472168</v>
       </c>
       <c r="F24" t="n">
         <v>1.0</v>
@@ -16914,19 +17114,19 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>27.0</v>
+        <v>7.0</v>
       </c>
       <c r="B25" t="n">
-        <v>15.0</v>
+        <v>19.0</v>
       </c>
       <c r="C25" t="n">
-        <v>8.0</v>
+        <v>26.419689178466797</v>
       </c>
       <c r="D25" t="n">
-        <v>6.338943043987854</v>
+        <v>336.359591450648</v>
       </c>
       <c r="E25" t="n">
-        <v>8.246211051940918</v>
+        <v>6.082762718200684</v>
       </c>
       <c r="F25" t="n">
         <v>1.0</v>
@@ -16934,19 +17134,19 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>6.0</v>
+        <v>26.0</v>
       </c>
       <c r="B26" t="n">
-        <v>15.0</v>
+        <v>7.0</v>
       </c>
       <c r="C26" t="n">
-        <v>11.401754379272461</v>
+        <v>28.160255432128906</v>
       </c>
       <c r="D26" t="n">
-        <v>152.0144894752111</v>
+        <v>164.42302223578986</v>
       </c>
       <c r="E26" t="n">
-        <v>9.05538558959961</v>
+        <v>11.180339813232422</v>
       </c>
       <c r="F26" t="n">
         <v>1.0</v>
@@ -16954,19 +17154,19 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>7.0</v>
+        <v>48.0</v>
       </c>
       <c r="B27" t="n">
-        <v>19.0</v>
+        <v>17.0</v>
       </c>
       <c r="C27" t="n">
-        <v>26.419689178466797</v>
+        <v>15.81138801574707</v>
       </c>
       <c r="D27" t="n">
-        <v>336.359591450648</v>
+        <v>315.2115326768105</v>
       </c>
       <c r="E27" t="n">
-        <v>16.492422103881836</v>
+        <v>13.152946472167969</v>
       </c>
       <c r="F27" t="n">
         <v>1.0</v>
@@ -16974,19 +17174,19 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>26.0</v>
+        <v>6.0</v>
       </c>
       <c r="B28" t="n">
-        <v>7.0</v>
+        <v>15.0</v>
       </c>
       <c r="C28" t="n">
-        <v>28.160255432128906</v>
+        <v>11.401754379272461</v>
       </c>
       <c r="D28" t="n">
-        <v>164.42302223578986</v>
+        <v>152.0144894752111</v>
       </c>
       <c r="E28" t="n">
-        <v>11.180339813232422</v>
+        <v>8.9442720413208</v>
       </c>
       <c r="F28" t="n">
         <v>1.0</v>
@@ -16994,19 +17194,19 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B29" t="n">
         <v>8.0</v>
       </c>
-      <c r="B29" t="n">
-        <v>23.0</v>
-      </c>
       <c r="C29" t="n">
-        <v>22.022714614868164</v>
+        <v>20.808652877807617</v>
       </c>
       <c r="D29" t="n">
-        <v>337.0548166268401</v>
+        <v>323.25993313398806</v>
       </c>
       <c r="E29" t="n">
-        <v>7.211102485656738</v>
+        <v>23.25940704345703</v>
       </c>
       <c r="F29" t="n">
         <v>1.0</v>
@@ -17014,19 +17214,19 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>22.0</v>
+        <v>31.0</v>
       </c>
       <c r="B30" t="n">
-        <v>8.0</v>
+        <v>11.0</v>
       </c>
       <c r="C30" t="n">
-        <v>20.808652877807617</v>
+        <v>29.832868576049805</v>
       </c>
       <c r="D30" t="n">
-        <v>323.25993313398806</v>
+        <v>353.7970010977599</v>
       </c>
       <c r="E30" t="n">
-        <v>12.083045959472656</v>
+        <v>13.0</v>
       </c>
       <c r="F30" t="n">
         <v>1.0</v>
@@ -17034,19 +17234,19 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>3.0</v>
+        <v>28.0</v>
       </c>
       <c r="B31" t="n">
-        <v>16.0</v>
+        <v>14.0</v>
       </c>
       <c r="C31" t="n">
-        <v>32.557640075683594</v>
+        <v>29.96664810180664</v>
       </c>
       <c r="D31" t="n">
-        <v>171.05352046358252</v>
+        <v>4.644742023417905</v>
       </c>
       <c r="E31" t="n">
-        <v>12.206555366516113</v>
+        <v>6.324555397033691</v>
       </c>
       <c r="F31" t="n">
         <v>1.0</v>
@@ -17066,7 +17266,7 @@
         <v>288.540600851905</v>
       </c>
       <c r="E32" t="n">
-        <v>12.083045959472656</v>
+        <v>20.099750518798828</v>
       </c>
       <c r="F32" t="n">
         <v>1.0</v>
@@ -17094,19 +17294,19 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>2.0</v>
+        <v>32.0</v>
       </c>
       <c r="B34" t="n">
-        <v>30.0</v>
+        <v>12.0</v>
       </c>
       <c r="C34" t="n">
-        <v>21.02379608154297</v>
+        <v>10.0</v>
       </c>
       <c r="D34" t="n">
-        <v>8.387652948531183</v>
+        <v>276.470003989416</v>
       </c>
       <c r="E34" t="n">
-        <v>12.041594505310059</v>
+        <v>22.472204208374023</v>
       </c>
       <c r="F34" t="n">
         <v>1.0</v>
@@ -17114,19 +17314,19 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>9.0</v>
+        <v>46.0</v>
       </c>
       <c r="B35" t="n">
-        <v>11.0</v>
+        <v>5.0</v>
       </c>
       <c r="C35" t="n">
-        <v>23.0867919921875</v>
+        <v>2.2360680103302</v>
       </c>
       <c r="D35" t="n">
-        <v>171.05352046358252</v>
+        <v>251.4270412434094</v>
       </c>
       <c r="E35" t="n">
-        <v>16.278820037841797</v>
+        <v>9.219544410705566</v>
       </c>
       <c r="F35" t="n">
         <v>1.0</v>
@@ -17134,19 +17334,19 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>30.0</v>
+        <v>51.0</v>
       </c>
       <c r="B36" t="n">
-        <v>19.0</v>
+        <v>160.0</v>
       </c>
       <c r="C36" t="n">
-        <v>30.870698928833008</v>
+        <v>0.0</v>
       </c>
       <c r="D36" t="n">
-        <v>187.07804971242513</v>
+        <v>6.338943043987854</v>
       </c>
       <c r="E36" t="n">
-        <v>8.485280990600586</v>
+        <v>2.2360680103302</v>
       </c>
       <c r="F36" t="n">
         <v>1.0</v>
@@ -17154,19 +17354,19 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>39.0</v>
+        <v>47.0</v>
       </c>
       <c r="B37" t="n">
-        <v>14.0</v>
+        <v>25.0</v>
       </c>
       <c r="C37" t="n">
-        <v>38.28837966918945</v>
+        <v>9.433980941772461</v>
       </c>
       <c r="D37" t="n">
-        <v>321.1319132345335</v>
+        <v>315.2115326768105</v>
       </c>
       <c r="E37" t="n">
-        <v>12.041594505310059</v>
+        <v>9.433980941772461</v>
       </c>
       <c r="F37" t="n">
         <v>1.0</v>
@@ -17174,19 +17374,19 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>49.0</v>
+        <v>12.0</v>
       </c>
       <c r="B38" t="n">
-        <v>18.0</v>
+        <v>29.0</v>
       </c>
       <c r="C38" t="n">
-        <v>21.63330841064453</v>
+        <v>8.062257766723633</v>
       </c>
       <c r="D38" t="n">
-        <v>304.9704733621193</v>
+        <v>337.0548166268401</v>
       </c>
       <c r="E38" t="n">
-        <v>17.029386520385742</v>
+        <v>6.0</v>
       </c>
       <c r="F38" t="n">
         <v>1.0</v>
@@ -17194,19 +17394,19 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>38.0</v>
+        <v>39.0</v>
       </c>
       <c r="B39" t="n">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="C39" t="n">
-        <v>15.81138801574707</v>
+        <v>38.28837966918945</v>
       </c>
       <c r="D39" t="n">
-        <v>216.59028435753538</v>
+        <v>321.1319132345335</v>
       </c>
       <c r="E39" t="n">
-        <v>7.6157732009887695</v>
+        <v>32.75667953491211</v>
       </c>
       <c r="F39" t="n">
         <v>1.0</v>
@@ -17214,19 +17414,19 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>5.0</v>
+        <v>33.0</v>
       </c>
       <c r="B40" t="n">
-        <v>21.0</v>
+        <v>23.0</v>
       </c>
       <c r="C40" t="n">
-        <v>14.142135620117188</v>
+        <v>34.0</v>
       </c>
       <c r="D40" t="n">
-        <v>360.0</v>
+        <v>157.54908042266146</v>
       </c>
       <c r="E40" t="n">
-        <v>7.071067810058594</v>
+        <v>13.928388595581055</v>
       </c>
       <c r="F40" t="n">
         <v>1.0</v>
@@ -17234,19 +17434,19 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>37.0</v>
+        <v>44.0</v>
       </c>
       <c r="B41" t="n">
-        <v>9.0</v>
+        <v>16.0</v>
       </c>
       <c r="C41" t="n">
-        <v>18.11077117919922</v>
+        <v>25.0</v>
       </c>
       <c r="D41" t="n">
-        <v>251.4270412434094</v>
+        <v>6.338943043987854</v>
       </c>
       <c r="E41" t="n">
-        <v>11.313708305358887</v>
+        <v>16.76305389404297</v>
       </c>
       <c r="F41" t="n">
         <v>1.0</v>
@@ -17254,19 +17454,19 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>15.0</v>
+        <v>4.0</v>
       </c>
       <c r="B42" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="C42" t="n">
-        <v>24.73863410949707</v>
+        <v>17.20465087890625</v>
       </c>
       <c r="D42" t="n">
-        <v>350.81816695114793</v>
+        <v>206.94372235198546</v>
       </c>
       <c r="E42" t="n">
-        <v>7.211102485656738</v>
+        <v>14.866068840026855</v>
       </c>
       <c r="F42" t="n">
         <v>1.0</v>
@@ -17274,19 +17474,19 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>44.0</v>
+        <v>42.0</v>
       </c>
       <c r="B43" t="n">
-        <v>16.0</v>
+        <v>13.0</v>
       </c>
       <c r="C43" t="n">
-        <v>25.0</v>
+        <v>31.320919036865234</v>
       </c>
       <c r="D43" t="n">
-        <v>6.338943043987854</v>
+        <v>152.0144894752111</v>
       </c>
       <c r="E43" t="n">
-        <v>6.082762718200684</v>
+        <v>16.031219482421875</v>
       </c>
       <c r="F43" t="n">
         <v>1.0</v>
@@ -17306,94 +17506,94 @@
         <v>303.7008314149076</v>
       </c>
       <c r="E44" t="n">
-        <v>33.541019439697266</v>
+        <v>23.25940704345703</v>
       </c>
       <c r="F44" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="s" s="55">
+      <c r="A45" t="s" s="103">
         <v>27</v>
       </c>
-      <c r="B45" s="59" t="n">
+      <c r="B45" s="107" t="n">
         <f>SUM(B18:B44)</f>
-        <v>520.0</v>
-      </c>
-      <c r="E45" s="59" t="n">
+        <v>540.0</v>
+      </c>
+      <c r="E45" s="107" t="n">
         <f>SUM(E18:E44)</f>
-        <v>301.8073661327362</v>
+        <v>362.7698333263397</v>
       </c>
     </row>
     <row r="46"/>
     <row r="47"/>
     <row r="48"/>
     <row r="49">
-      <c r="A49" t="s" s="55">
+      <c r="A49" t="s" s="103">
         <v>10</v>
       </c>
-      <c r="B49" t="n" s="56">
+      <c r="B49" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="C49" t="s" s="55">
+      <c r="C49" t="s" s="103">
         <v>11</v>
       </c>
-      <c r="D49" t="n" s="56">
+      <c r="D49" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="E49" t="s" s="55">
+      <c r="E49" t="s" s="103">
         <v>12</v>
       </c>
-      <c r="F49" t="n" s="56">
+      <c r="F49" t="n" s="104">
         <v>-1.0</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s" s="55">
+      <c r="A50" t="s" s="103">
         <v>13</v>
       </c>
-      <c r="B50" t="n" s="56">
+      <c r="B50" t="n" s="104">
         <v>1.0</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="s" s="55">
+      <c r="A51" t="s" s="103">
         <v>14</v>
       </c>
-      <c r="B51" t="n" s="56">
+      <c r="B51" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="C51" t="s" s="55">
+      <c r="C51" t="s" s="103">
         <v>15</v>
       </c>
-      <c r="D51" t="n" s="56">
+      <c r="D51" t="n" s="104">
         <v>160.0</v>
       </c>
-      <c r="E51" t="s" s="55">
+      <c r="E51" t="s" s="103">
         <v>16</v>
       </c>
-      <c r="F51" t="n" s="60">
-        <v>417.0</v>
+      <c r="F51" t="n" s="108">
+        <v>397.0</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="s" s="55">
+      <c r="A52" t="s" s="103">
         <v>17</v>
       </c>
-      <c r="B52" t="n" s="56">
-        <v>3.555601966640625E9</v>
-      </c>
-      <c r="C52" t="s" s="55">
+      <c r="B52" t="n" s="104">
+        <v>3.1029216077539062E9</v>
+      </c>
+      <c r="C52" t="s" s="103">
         <v>18</v>
       </c>
-      <c r="D52" t="n" s="56">
+      <c r="D52" t="n" s="104">
         <v>9999999.0</v>
       </c>
-      <c r="E52" t="s" s="55">
+      <c r="E52" t="s" s="103">
         <v>19</v>
       </c>
-      <c r="F52" t="n" s="59">
-        <v>355.5601806640625</v>
+      <c r="F52" t="n" s="107">
+        <v>310.2921447753906</v>
       </c>
     </row>
     <row r="53"/>
@@ -17439,19 +17639,19 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>19.0</v>
+        <v>45.0</v>
       </c>
       <c r="B56" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="C56" t="n">
-        <v>31.906112670898438</v>
+        <v>31.320919036865234</v>
       </c>
       <c r="D56" t="n">
-        <v>264.5569058120526</v>
+        <v>196.6523324938246</v>
       </c>
       <c r="E56" t="n">
-        <v>18.384777069091797</v>
+        <v>40.26164245605469</v>
       </c>
       <c r="F56" t="n">
         <v>1.0</v>
@@ -17459,19 +17659,19 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>42.0</v>
+        <v>15.0</v>
       </c>
       <c r="B57" t="n">
-        <v>13.0</v>
+        <v>10.0</v>
       </c>
       <c r="C57" t="n">
-        <v>31.320919036865234</v>
+        <v>24.73863410949707</v>
       </c>
       <c r="D57" t="n">
-        <v>152.0144894752111</v>
+        <v>350.81816695114793</v>
       </c>
       <c r="E57" t="n">
-        <v>8.5440034866333</v>
+        <v>6.7082037925720215</v>
       </c>
       <c r="F57" t="n">
         <v>1.0</v>
@@ -17479,19 +17679,19 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>17.0</v>
+        <v>5.0</v>
       </c>
       <c r="B58" t="n">
-        <v>3.0</v>
+        <v>21.0</v>
       </c>
       <c r="C58" t="n">
-        <v>17.262676239013672</v>
+        <v>14.142135620117188</v>
       </c>
       <c r="D58" t="n">
-        <v>164.42302223578986</v>
+        <v>360.0</v>
       </c>
       <c r="E58" t="n">
-        <v>14.317821502685547</v>
+        <v>14.560219764709473</v>
       </c>
       <c r="F58" t="n">
         <v>1.0</v>
@@ -17499,19 +17699,19 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>45.0</v>
+        <v>49.0</v>
       </c>
       <c r="B59" t="n">
-        <v>10.0</v>
+        <v>18.0</v>
       </c>
       <c r="C59" t="n">
-        <v>31.320919036865234</v>
+        <v>21.63330841064453</v>
       </c>
       <c r="D59" t="n">
-        <v>196.6523324938246</v>
+        <v>304.9704733621193</v>
       </c>
       <c r="E59" t="n">
-        <v>17.69180679321289</v>
+        <v>8.246211051940918</v>
       </c>
       <c r="F59" t="n">
         <v>1.0</v>
@@ -17519,19 +17719,19 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>33.0</v>
+        <v>10.0</v>
       </c>
       <c r="B60" t="n">
-        <v>23.0</v>
+        <v>5.0</v>
       </c>
       <c r="C60" t="n">
-        <v>34.0</v>
+        <v>28.319604873657227</v>
       </c>
       <c r="D60" t="n">
-        <v>157.54908042266146</v>
+        <v>238.80064659365183</v>
       </c>
       <c r="E60" t="n">
-        <v>7.0</v>
+        <v>7.6157732009887695</v>
       </c>
       <c r="F60" t="n">
         <v>1.0</v>
@@ -17539,19 +17739,19 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>10.0</v>
+        <v>30.0</v>
       </c>
       <c r="B61" t="n">
-        <v>5.0</v>
+        <v>19.0</v>
       </c>
       <c r="C61" t="n">
-        <v>28.319604873657227</v>
+        <v>30.870698928833008</v>
       </c>
       <c r="D61" t="n">
-        <v>238.80064659365183</v>
+        <v>187.07804971242513</v>
       </c>
       <c r="E61" t="n">
-        <v>12.083045959472656</v>
+        <v>9.219544410705566</v>
       </c>
       <c r="F61" t="n">
         <v>1.0</v>
@@ -17559,19 +17759,19 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>34.0</v>
+        <v>9.0</v>
       </c>
       <c r="B62" t="n">
-        <v>26.0</v>
+        <v>11.0</v>
       </c>
       <c r="C62" t="n">
-        <v>31.78049659729004</v>
+        <v>23.0867919921875</v>
       </c>
       <c r="D62" t="n">
-        <v>338.16739400253954</v>
+        <v>171.05352046358252</v>
       </c>
       <c r="E62" t="n">
-        <v>15.620499610900879</v>
+        <v>8.485280990600586</v>
       </c>
       <c r="F62" t="n">
         <v>1.0</v>
@@ -17591,7 +17791,7 @@
         <v>345.5992243656941</v>
       </c>
       <c r="E63" t="n">
-        <v>6.4031243324279785</v>
+        <v>5.656854152679443</v>
       </c>
       <c r="F63" t="n">
         <v>1.0</v>
@@ -17599,19 +17799,19 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>21.0</v>
+        <v>34.0</v>
       </c>
       <c r="B64" t="n">
-        <v>8.0</v>
+        <v>26.0</v>
       </c>
       <c r="C64" t="n">
-        <v>32.06243896484375</v>
+        <v>31.78049659729004</v>
       </c>
       <c r="D64" t="n">
-        <v>359.656656935923</v>
+        <v>338.16739400253954</v>
       </c>
       <c r="E64" t="n">
-        <v>7.8102498054504395</v>
+        <v>6.4031243324279785</v>
       </c>
       <c r="F64" t="n">
         <v>1.0</v>
@@ -17619,19 +17819,19 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>29.0</v>
+        <v>21.0</v>
       </c>
       <c r="B65" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="C65" t="n">
-        <v>29.120439529418945</v>
+        <v>32.06243896484375</v>
       </c>
       <c r="D65" t="n">
-        <v>187.07804971242513</v>
+        <v>359.656656935923</v>
       </c>
       <c r="E65" t="n">
-        <v>7.211102485656738</v>
+        <v>9.05538558959961</v>
       </c>
       <c r="F65" t="n">
         <v>1.0</v>
@@ -17639,19 +17839,19 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>16.0</v>
+        <v>29.0</v>
       </c>
       <c r="B66" t="n">
-        <v>15.0</v>
+        <v>6.0</v>
       </c>
       <c r="C66" t="n">
-        <v>22.022714614868164</v>
+        <v>29.120439529418945</v>
       </c>
       <c r="D66" t="n">
-        <v>171.05352046358252</v>
+        <v>187.07804971242513</v>
       </c>
       <c r="E66" t="n">
-        <v>9.219544410705566</v>
+        <v>7.211102485656738</v>
       </c>
       <c r="F66" t="n">
         <v>1.0</v>
@@ -17659,19 +17859,19 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>11.0</v>
+        <v>16.0</v>
       </c>
       <c r="B67" t="n">
-        <v>19.0</v>
+        <v>15.0</v>
       </c>
       <c r="C67" t="n">
-        <v>12.041594505310059</v>
+        <v>22.022714614868164</v>
       </c>
       <c r="D67" t="n">
-        <v>323.25993313398806</v>
+        <v>171.05352046358252</v>
       </c>
       <c r="E67" t="n">
-        <v>10.0</v>
+        <v>9.219544410705566</v>
       </c>
       <c r="F67" t="n">
         <v>1.0</v>
@@ -17679,19 +17879,19 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>35.0</v>
+        <v>2.0</v>
       </c>
       <c r="B68" t="n">
-        <v>17.0</v>
+        <v>30.0</v>
       </c>
       <c r="C68" t="n">
-        <v>39.408119201660156</v>
+        <v>21.02379608154297</v>
       </c>
       <c r="D68" t="n">
-        <v>359.656656935923</v>
+        <v>8.387652948531183</v>
       </c>
       <c r="E68" t="n">
-        <v>29.73213768005371</v>
+        <v>8.5440034866333</v>
       </c>
       <c r="F68" t="n">
         <v>1.0</v>
@@ -17699,19 +17899,19 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>28.0</v>
+        <v>35.0</v>
       </c>
       <c r="B69" t="n">
-        <v>14.0</v>
+        <v>17.0</v>
       </c>
       <c r="C69" t="n">
-        <v>29.96664810180664</v>
+        <v>39.408119201660156</v>
       </c>
       <c r="D69" t="n">
-        <v>4.644742023417905</v>
+        <v>359.656656935923</v>
       </c>
       <c r="E69" t="n">
-        <v>19.416488647460938</v>
+        <v>19.10497283935547</v>
       </c>
       <c r="F69" t="n">
         <v>1.0</v>
@@ -17719,19 +17919,19 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>31.0</v>
+        <v>3.0</v>
       </c>
       <c r="B70" t="n">
-        <v>11.0</v>
+        <v>16.0</v>
       </c>
       <c r="C70" t="n">
-        <v>29.832868576049805</v>
+        <v>32.557640075683594</v>
       </c>
       <c r="D70" t="n">
-        <v>353.7970010977599</v>
+        <v>171.05352046358252</v>
       </c>
       <c r="E70" t="n">
-        <v>6.324555397033691</v>
+        <v>10.049875259399414</v>
       </c>
       <c r="F70" t="n">
         <v>1.0</v>
@@ -17739,19 +17939,19 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="B71" t="n">
-        <v>7.0</v>
+        <v>23.0</v>
       </c>
       <c r="C71" t="n">
-        <v>13.892443656921387</v>
+        <v>22.022714614868164</v>
       </c>
       <c r="D71" t="n">
-        <v>353.7970010977599</v>
+        <v>337.0548166268401</v>
       </c>
       <c r="E71" t="n">
-        <v>17.0</v>
+        <v>21.095022201538086</v>
       </c>
       <c r="F71" t="n">
         <v>1.0</v>
@@ -17759,19 +17959,19 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
       <c r="B72" t="n">
-        <v>29.0</v>
+        <v>7.0</v>
       </c>
       <c r="C72" t="n">
-        <v>8.062257766723633</v>
+        <v>13.892443656921387</v>
       </c>
       <c r="D72" t="n">
-        <v>337.0548166268401</v>
+        <v>353.7970010977599</v>
       </c>
       <c r="E72" t="n">
-        <v>20.880613327026367</v>
+        <v>11.661903381347656</v>
       </c>
       <c r="F72" t="n">
         <v>1.0</v>
@@ -17779,19 +17979,19 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>47.0</v>
+        <v>27.0</v>
       </c>
       <c r="B73" t="n">
-        <v>25.0</v>
+        <v>15.0</v>
       </c>
       <c r="C73" t="n">
-        <v>9.433980941772461</v>
+        <v>8.0</v>
       </c>
       <c r="D73" t="n">
-        <v>315.2115326768105</v>
+        <v>6.338943043987854</v>
       </c>
       <c r="E73" t="n">
-        <v>6.0</v>
+        <v>8.062257766723633</v>
       </c>
       <c r="F73" t="n">
         <v>1.0</v>
@@ -17799,19 +17999,19 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>18.0</v>
+        <v>11.0</v>
       </c>
       <c r="B74" t="n">
-        <v>41.0</v>
+        <v>19.0</v>
       </c>
       <c r="C74" t="n">
-        <v>14.764822959899902</v>
+        <v>12.041594505310059</v>
       </c>
       <c r="D74" t="n">
-        <v>336.359591450648</v>
+        <v>323.25993313398806</v>
       </c>
       <c r="E74" t="n">
-        <v>8.062257766723633</v>
+        <v>13.892443656921387</v>
       </c>
       <c r="F74" t="n">
         <v>1.0</v>
@@ -17819,19 +18019,19 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>48.0</v>
+        <v>38.0</v>
       </c>
       <c r="B75" t="n">
-        <v>17.0</v>
+        <v>15.0</v>
       </c>
       <c r="C75" t="n">
         <v>15.81138801574707</v>
       </c>
       <c r="D75" t="n">
-        <v>315.2115326768105</v>
+        <v>216.59028435753538</v>
       </c>
       <c r="E75" t="n">
-        <v>23.409399032592773</v>
+        <v>6.7082037925720215</v>
       </c>
       <c r="F75" t="n">
         <v>1.0</v>
@@ -17839,19 +18039,19 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>23.0</v>
+        <v>37.0</v>
       </c>
       <c r="B76" t="n">
-        <v>16.0</v>
+        <v>9.0</v>
       </c>
       <c r="C76" t="n">
-        <v>22.022714614868164</v>
+        <v>18.11077117919922</v>
       </c>
       <c r="D76" t="n">
-        <v>299.7015117237478</v>
+        <v>251.4270412434094</v>
       </c>
       <c r="E76" t="n">
-        <v>9.219544410705566</v>
+        <v>18.384777069091797</v>
       </c>
       <c r="F76" t="n">
         <v>1.0</v>
@@ -17859,19 +18059,19 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>43.0</v>
+        <v>17.0</v>
       </c>
       <c r="B77" t="n">
-        <v>11.0</v>
+        <v>3.0</v>
       </c>
       <c r="C77" t="n">
-        <v>34.65544509887695</v>
+        <v>17.262676239013672</v>
       </c>
       <c r="D77" t="n">
-        <v>8.319952741629265</v>
+        <v>164.42302223578986</v>
       </c>
       <c r="E77" t="n">
-        <v>13.03840446472168</v>
+        <v>5.099019527435303</v>
       </c>
       <c r="F77" t="n">
         <v>1.0</v>
@@ -17879,19 +18079,19 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>24.0</v>
+        <v>18.0</v>
       </c>
       <c r="B78" t="n">
-        <v>10.0</v>
+        <v>41.0</v>
       </c>
       <c r="C78" t="n">
-        <v>25.05992889404297</v>
+        <v>14.764822959899902</v>
       </c>
       <c r="D78" t="n">
-        <v>171.97940109631875</v>
+        <v>336.359591450648</v>
       </c>
       <c r="E78" t="n">
-        <v>12.369317054748535</v>
+        <v>14.142135620117188</v>
       </c>
       <c r="F78" t="n">
         <v>1.0</v>
@@ -17899,19 +18099,19 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
       </c>
       <c r="B79" t="n">
-        <v>21.0</v>
+        <v>27.0</v>
       </c>
       <c r="C79" t="n">
-        <v>18.11077117919922</v>
+        <v>30.479501724243164</v>
       </c>
       <c r="D79" t="n">
-        <v>346.6473834054614</v>
+        <v>298.9856443268601</v>
       </c>
       <c r="E79" t="n">
-        <v>10.770329475402832</v>
+        <v>17.464248657226562</v>
       </c>
       <c r="F79" t="n">
         <v>1.0</v>
@@ -17919,19 +18119,19 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>25.0</v>
+        <v>19.0</v>
       </c>
       <c r="B80" t="n">
-        <v>28.0</v>
+        <v>9.0</v>
       </c>
       <c r="C80" t="n">
-        <v>23.0867919921875</v>
+        <v>31.906112670898438</v>
       </c>
       <c r="D80" t="n">
-        <v>240.25810175410237</v>
+        <v>264.5569058120526</v>
       </c>
       <c r="E80" t="n">
-        <v>6.4031243324279785</v>
+        <v>5.0</v>
       </c>
       <c r="F80" t="n">
         <v>1.0</v>
@@ -17939,19 +18139,19 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>13.0</v>
+        <v>40.0</v>
       </c>
       <c r="B81" t="n">
-        <v>23.0</v>
+        <v>7.0</v>
       </c>
       <c r="C81" t="n">
-        <v>29.154760360717773</v>
+        <v>42.20189666748047</v>
       </c>
       <c r="D81" t="n">
         <v>8.319952741629265</v>
       </c>
       <c r="E81" t="n">
-        <v>13.152946472167969</v>
+        <v>10.630146026611328</v>
       </c>
       <c r="F81" t="n">
         <v>1.0</v>
@@ -17971,94 +18171,94 @@
         <v>303.7008314149076</v>
       </c>
       <c r="E82" t="n">
-        <v>25.495098114013672</v>
+        <v>7.8102498054504395</v>
       </c>
       <c r="F82" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="s" s="55">
+      <c r="A83" t="s" s="103">
         <v>27</v>
       </c>
-      <c r="B83" s="59" t="n">
+      <c r="B83" s="107" t="n">
         <f>SUM(B55:B82)</f>
-        <v>417.0</v>
-      </c>
-      <c r="E83" s="59" t="n">
+        <v>397.0</v>
+      </c>
+      <c r="E83" s="107" t="n">
         <f>SUM(E55:E82)</f>
-        <v>355.56019163131714</v>
+        <v>310.29214572906494</v>
       </c>
     </row>
     <row r="84"/>
     <row r="85"/>
     <row r="86"/>
     <row r="87">
-      <c r="A87" t="s" s="55">
+      <c r="A87" t="s" s="103">
         <v>10</v>
       </c>
-      <c r="B87" t="n" s="56">
+      <c r="B87" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="C87" t="s" s="55">
+      <c r="C87" t="s" s="103">
         <v>11</v>
       </c>
-      <c r="D87" t="n" s="56">
+      <c r="D87" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="E87" t="s" s="55">
+      <c r="E87" t="s" s="103">
         <v>12</v>
       </c>
-      <c r="F87" t="n" s="56">
+      <c r="F87" t="n" s="104">
         <v>-1.0</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="s" s="55">
+      <c r="A88" t="s" s="103">
         <v>13</v>
       </c>
-      <c r="B88" t="n" s="56">
+      <c r="B88" t="n" s="104">
         <v>0.0</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="s" s="55">
+      <c r="A89" t="s" s="103">
         <v>14</v>
       </c>
-      <c r="B89" t="n" s="56">
+      <c r="B89" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="C89" t="s" s="55">
+      <c r="C89" t="s" s="103">
         <v>15</v>
       </c>
-      <c r="D89" t="n" s="56">
+      <c r="D89" t="n" s="104">
         <v>160.0</v>
       </c>
-      <c r="E89" t="s" s="55">
+      <c r="E89" t="s" s="103">
         <v>16</v>
       </c>
-      <c r="F89" t="n" s="60">
-        <v>520.0</v>
+      <c r="F89" t="n" s="108">
+        <v>540.0</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="s" s="55">
+      <c r="A90" t="s" s="103">
         <v>17</v>
       </c>
-      <c r="B90" t="n" s="56">
-        <v>3.0180735852929688E9</v>
-      </c>
-      <c r="C90" t="s" s="55">
+      <c r="B90" t="n" s="104">
+        <v>3.6276982190820312E9</v>
+      </c>
+      <c r="C90" t="s" s="103">
         <v>18</v>
       </c>
-      <c r="D90" t="n" s="56">
+      <c r="D90" t="n" s="104">
         <v>9999999.0</v>
       </c>
-      <c r="E90" t="s" s="55">
+      <c r="E90" t="s" s="103">
         <v>19</v>
       </c>
-      <c r="F90" t="n" s="59">
-        <v>301.8073425292969</v>
+      <c r="F90" t="n" s="107">
+        <v>362.7698059082031</v>
       </c>
     </row>
     <row r="91"/>
@@ -18104,19 +18304,19 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>40.0</v>
+        <v>13.0</v>
       </c>
       <c r="B94" t="n">
-        <v>7.0</v>
+        <v>23.0</v>
       </c>
       <c r="C94" t="n">
-        <v>42.20189666748047</v>
+        <v>29.154760360717773</v>
       </c>
       <c r="D94" t="n">
         <v>8.319952741629265</v>
       </c>
       <c r="E94" t="n">
-        <v>7.8102498054504395</v>
+        <v>25.495098114013672</v>
       </c>
       <c r="F94" t="n">
         <v>1.0</v>
@@ -18124,19 +18324,19 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>41.0</v>
+        <v>25.0</v>
       </c>
       <c r="B95" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="C95" t="n">
-        <v>30.479501724243164</v>
+        <v>23.0867919921875</v>
       </c>
       <c r="D95" t="n">
-        <v>298.9856443268601</v>
+        <v>240.25810175410237</v>
       </c>
       <c r="E95" t="n">
-        <v>12.083045959472656</v>
+        <v>13.152946472167969</v>
       </c>
       <c r="F95" t="n">
         <v>1.0</v>
@@ -18144,19 +18344,19 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>4.0</v>
+        <v>14.0</v>
       </c>
       <c r="B96" t="n">
-        <v>9.0</v>
+        <v>21.0</v>
       </c>
       <c r="C96" t="n">
-        <v>17.20465087890625</v>
+        <v>18.11077117919922</v>
       </c>
       <c r="D96" t="n">
-        <v>206.94372235198546</v>
+        <v>346.6473834054614</v>
       </c>
       <c r="E96" t="n">
-        <v>13.45362377166748</v>
+        <v>6.4031243324279785</v>
       </c>
       <c r="F96" t="n">
         <v>1.0</v>
@@ -18164,19 +18364,19 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>51.0</v>
+        <v>24.0</v>
       </c>
       <c r="B97" t="n">
-        <v>160.0</v>
+        <v>10.0</v>
       </c>
       <c r="C97" t="n">
-        <v>0.0</v>
+        <v>25.05992889404297</v>
       </c>
       <c r="D97" t="n">
-        <v>6.338943043987854</v>
+        <v>171.97940109631875</v>
       </c>
       <c r="E97" t="n">
-        <v>17.20465087890625</v>
+        <v>10.770329475402832</v>
       </c>
       <c r="F97" t="n">
         <v>1.0</v>
@@ -18184,19 +18384,19 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>46.0</v>
+        <v>43.0</v>
       </c>
       <c r="B98" t="n">
-        <v>5.0</v>
+        <v>11.0</v>
       </c>
       <c r="C98" t="n">
-        <v>2.2360680103302</v>
+        <v>34.65544509887695</v>
       </c>
       <c r="D98" t="n">
-        <v>251.4270412434094</v>
+        <v>8.319952741629265</v>
       </c>
       <c r="E98" t="n">
-        <v>2.2360680103302</v>
+        <v>12.369317054748535</v>
       </c>
       <c r="F98" t="n">
         <v>1.0</v>
@@ -18204,19 +18404,19 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>32.0</v>
+        <v>23.0</v>
       </c>
       <c r="B99" t="n">
-        <v>12.0</v>
+        <v>16.0</v>
       </c>
       <c r="C99" t="n">
-        <v>10.0</v>
+        <v>22.022714614868164</v>
       </c>
       <c r="D99" t="n">
-        <v>276.470003989416</v>
+        <v>299.7015117237478</v>
       </c>
       <c r="E99" t="n">
-        <v>9.219544410705566</v>
+        <v>13.03840446472168</v>
       </c>
       <c r="F99" t="n">
         <v>1.0</v>
@@ -18224,19 +18424,19 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>27.0</v>
+        <v>7.0</v>
       </c>
       <c r="B100" t="n">
-        <v>15.0</v>
+        <v>19.0</v>
       </c>
       <c r="C100" t="n">
-        <v>8.0</v>
+        <v>26.419689178466797</v>
       </c>
       <c r="D100" t="n">
-        <v>6.338943043987854</v>
+        <v>336.359591450648</v>
       </c>
       <c r="E100" t="n">
-        <v>8.246211051940918</v>
+        <v>6.082762718200684</v>
       </c>
       <c r="F100" t="n">
         <v>1.0</v>
@@ -18244,19 +18444,19 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>6.0</v>
+        <v>26.0</v>
       </c>
       <c r="B101" t="n">
-        <v>15.0</v>
+        <v>7.0</v>
       </c>
       <c r="C101" t="n">
-        <v>11.401754379272461</v>
+        <v>28.160255432128906</v>
       </c>
       <c r="D101" t="n">
-        <v>152.0144894752111</v>
+        <v>164.42302223578986</v>
       </c>
       <c r="E101" t="n">
-        <v>9.05538558959961</v>
+        <v>11.180339813232422</v>
       </c>
       <c r="F101" t="n">
         <v>1.0</v>
@@ -18264,19 +18464,19 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>7.0</v>
+        <v>48.0</v>
       </c>
       <c r="B102" t="n">
-        <v>19.0</v>
+        <v>17.0</v>
       </c>
       <c r="C102" t="n">
-        <v>26.419689178466797</v>
+        <v>15.81138801574707</v>
       </c>
       <c r="D102" t="n">
-        <v>336.359591450648</v>
+        <v>315.2115326768105</v>
       </c>
       <c r="E102" t="n">
-        <v>16.492422103881836</v>
+        <v>13.152946472167969</v>
       </c>
       <c r="F102" t="n">
         <v>1.0</v>
@@ -18284,19 +18484,19 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>26.0</v>
+        <v>6.0</v>
       </c>
       <c r="B103" t="n">
-        <v>7.0</v>
+        <v>15.0</v>
       </c>
       <c r="C103" t="n">
-        <v>28.160255432128906</v>
+        <v>11.401754379272461</v>
       </c>
       <c r="D103" t="n">
-        <v>164.42302223578986</v>
+        <v>152.0144894752111</v>
       </c>
       <c r="E103" t="n">
-        <v>11.180339813232422</v>
+        <v>8.9442720413208</v>
       </c>
       <c r="F103" t="n">
         <v>1.0</v>
@@ -18304,19 +18504,19 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B104" t="n">
         <v>8.0</v>
       </c>
-      <c r="B104" t="n">
-        <v>23.0</v>
-      </c>
       <c r="C104" t="n">
-        <v>22.022714614868164</v>
+        <v>20.808652877807617</v>
       </c>
       <c r="D104" t="n">
-        <v>337.0548166268401</v>
+        <v>323.25993313398806</v>
       </c>
       <c r="E104" t="n">
-        <v>7.211102485656738</v>
+        <v>23.25940704345703</v>
       </c>
       <c r="F104" t="n">
         <v>1.0</v>
@@ -18324,19 +18524,19 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>22.0</v>
+        <v>31.0</v>
       </c>
       <c r="B105" t="n">
-        <v>8.0</v>
+        <v>11.0</v>
       </c>
       <c r="C105" t="n">
-        <v>20.808652877807617</v>
+        <v>29.832868576049805</v>
       </c>
       <c r="D105" t="n">
-        <v>323.25993313398806</v>
+        <v>353.7970010977599</v>
       </c>
       <c r="E105" t="n">
-        <v>12.083045959472656</v>
+        <v>13.0</v>
       </c>
       <c r="F105" t="n">
         <v>1.0</v>
@@ -18344,19 +18544,19 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>3.0</v>
+        <v>28.0</v>
       </c>
       <c r="B106" t="n">
-        <v>16.0</v>
+        <v>14.0</v>
       </c>
       <c r="C106" t="n">
-        <v>32.557640075683594</v>
+        <v>29.96664810180664</v>
       </c>
       <c r="D106" t="n">
-        <v>171.05352046358252</v>
+        <v>4.644742023417905</v>
       </c>
       <c r="E106" t="n">
-        <v>12.206555366516113</v>
+        <v>6.324555397033691</v>
       </c>
       <c r="F106" t="n">
         <v>1.0</v>
@@ -18376,7 +18576,7 @@
         <v>288.540600851905</v>
       </c>
       <c r="E107" t="n">
-        <v>12.083045959472656</v>
+        <v>20.099750518798828</v>
       </c>
       <c r="F107" t="n">
         <v>1.0</v>
@@ -18404,19 +18604,19 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>2.0</v>
+        <v>32.0</v>
       </c>
       <c r="B109" t="n">
-        <v>30.0</v>
+        <v>12.0</v>
       </c>
       <c r="C109" t="n">
-        <v>21.02379608154297</v>
+        <v>10.0</v>
       </c>
       <c r="D109" t="n">
-        <v>8.387652948531183</v>
+        <v>276.470003989416</v>
       </c>
       <c r="E109" t="n">
-        <v>12.041594505310059</v>
+        <v>22.472204208374023</v>
       </c>
       <c r="F109" t="n">
         <v>1.0</v>
@@ -18424,19 +18624,19 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>9.0</v>
+        <v>46.0</v>
       </c>
       <c r="B110" t="n">
-        <v>11.0</v>
+        <v>5.0</v>
       </c>
       <c r="C110" t="n">
-        <v>23.0867919921875</v>
+        <v>2.2360680103302</v>
       </c>
       <c r="D110" t="n">
-        <v>171.05352046358252</v>
+        <v>251.4270412434094</v>
       </c>
       <c r="E110" t="n">
-        <v>16.278820037841797</v>
+        <v>9.219544410705566</v>
       </c>
       <c r="F110" t="n">
         <v>1.0</v>
@@ -18444,19 +18644,19 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>30.0</v>
+        <v>51.0</v>
       </c>
       <c r="B111" t="n">
-        <v>19.0</v>
+        <v>160.0</v>
       </c>
       <c r="C111" t="n">
-        <v>30.870698928833008</v>
+        <v>0.0</v>
       </c>
       <c r="D111" t="n">
-        <v>187.07804971242513</v>
+        <v>6.338943043987854</v>
       </c>
       <c r="E111" t="n">
-        <v>8.485280990600586</v>
+        <v>2.2360680103302</v>
       </c>
       <c r="F111" t="n">
         <v>1.0</v>
@@ -18464,19 +18664,19 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>39.0</v>
+        <v>47.0</v>
       </c>
       <c r="B112" t="n">
-        <v>14.0</v>
+        <v>25.0</v>
       </c>
       <c r="C112" t="n">
-        <v>38.28837966918945</v>
+        <v>9.433980941772461</v>
       </c>
       <c r="D112" t="n">
-        <v>321.1319132345335</v>
+        <v>315.2115326768105</v>
       </c>
       <c r="E112" t="n">
-        <v>12.041594505310059</v>
+        <v>9.433980941772461</v>
       </c>
       <c r="F112" t="n">
         <v>1.0</v>
@@ -18484,19 +18684,19 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>49.0</v>
+        <v>12.0</v>
       </c>
       <c r="B113" t="n">
-        <v>18.0</v>
+        <v>29.0</v>
       </c>
       <c r="C113" t="n">
-        <v>21.63330841064453</v>
+        <v>8.062257766723633</v>
       </c>
       <c r="D113" t="n">
-        <v>304.9704733621193</v>
+        <v>337.0548166268401</v>
       </c>
       <c r="E113" t="n">
-        <v>17.029386520385742</v>
+        <v>6.0</v>
       </c>
       <c r="F113" t="n">
         <v>1.0</v>
@@ -18504,19 +18704,19 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>38.0</v>
+        <v>39.0</v>
       </c>
       <c r="B114" t="n">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="C114" t="n">
-        <v>15.81138801574707</v>
+        <v>38.28837966918945</v>
       </c>
       <c r="D114" t="n">
-        <v>216.59028435753538</v>
+        <v>321.1319132345335</v>
       </c>
       <c r="E114" t="n">
-        <v>7.6157732009887695</v>
+        <v>32.75667953491211</v>
       </c>
       <c r="F114" t="n">
         <v>1.0</v>
@@ -18524,19 +18724,19 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>5.0</v>
+        <v>33.0</v>
       </c>
       <c r="B115" t="n">
-        <v>21.0</v>
+        <v>23.0</v>
       </c>
       <c r="C115" t="n">
-        <v>14.142135620117188</v>
+        <v>34.0</v>
       </c>
       <c r="D115" t="n">
-        <v>360.0</v>
+        <v>157.54908042266146</v>
       </c>
       <c r="E115" t="n">
-        <v>7.071067810058594</v>
+        <v>13.928388595581055</v>
       </c>
       <c r="F115" t="n">
         <v>1.0</v>
@@ -18544,19 +18744,19 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>37.0</v>
+        <v>44.0</v>
       </c>
       <c r="B116" t="n">
-        <v>9.0</v>
+        <v>16.0</v>
       </c>
       <c r="C116" t="n">
-        <v>18.11077117919922</v>
+        <v>25.0</v>
       </c>
       <c r="D116" t="n">
-        <v>251.4270412434094</v>
+        <v>6.338943043987854</v>
       </c>
       <c r="E116" t="n">
-        <v>11.313708305358887</v>
+        <v>16.76305389404297</v>
       </c>
       <c r="F116" t="n">
         <v>1.0</v>
@@ -18564,19 +18764,19 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>15.0</v>
+        <v>4.0</v>
       </c>
       <c r="B117" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="C117" t="n">
-        <v>24.73863410949707</v>
+        <v>17.20465087890625</v>
       </c>
       <c r="D117" t="n">
-        <v>350.81816695114793</v>
+        <v>206.94372235198546</v>
       </c>
       <c r="E117" t="n">
-        <v>7.211102485656738</v>
+        <v>14.866068840026855</v>
       </c>
       <c r="F117" t="n">
         <v>1.0</v>
@@ -18584,19 +18784,19 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>44.0</v>
+        <v>42.0</v>
       </c>
       <c r="B118" t="n">
-        <v>16.0</v>
+        <v>13.0</v>
       </c>
       <c r="C118" t="n">
-        <v>25.0</v>
+        <v>31.320919036865234</v>
       </c>
       <c r="D118" t="n">
-        <v>6.338943043987854</v>
+        <v>152.0144894752111</v>
       </c>
       <c r="E118" t="n">
-        <v>6.082762718200684</v>
+        <v>16.031219482421875</v>
       </c>
       <c r="F118" t="n">
         <v>1.0</v>
@@ -18616,94 +18816,94 @@
         <v>303.7008314149076</v>
       </c>
       <c r="E119" t="n">
-        <v>33.541019439697266</v>
+        <v>23.25940704345703</v>
       </c>
       <c r="F119" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="s" s="55">
+      <c r="A120" t="s" s="103">
         <v>27</v>
       </c>
-      <c r="B120" s="59" t="n">
+      <c r="B120" s="107" t="n">
         <f>SUM(B93:B119)</f>
-        <v>520.0</v>
-      </c>
-      <c r="E120" s="59" t="n">
+        <v>540.0</v>
+      </c>
+      <c r="E120" s="107" t="n">
         <f>SUM(E93:E119)</f>
-        <v>301.8073661327362</v>
+        <v>362.7698333263397</v>
       </c>
     </row>
     <row r="121"/>
     <row r="122"/>
     <row r="123"/>
     <row r="124">
-      <c r="A124" t="s" s="55">
+      <c r="A124" t="s" s="103">
         <v>10</v>
       </c>
-      <c r="B124" t="n" s="56">
+      <c r="B124" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="C124" t="s" s="55">
+      <c r="C124" t="s" s="103">
         <v>11</v>
       </c>
-      <c r="D124" t="n" s="56">
+      <c r="D124" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="E124" t="s" s="55">
+      <c r="E124" t="s" s="103">
         <v>12</v>
       </c>
-      <c r="F124" t="n" s="56">
+      <c r="F124" t="n" s="104">
         <v>-1.0</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="s" s="55">
+      <c r="A125" t="s" s="103">
         <v>13</v>
       </c>
-      <c r="B125" t="n" s="56">
+      <c r="B125" t="n" s="104">
         <v>1.0</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="s" s="55">
+      <c r="A126" t="s" s="103">
         <v>14</v>
       </c>
-      <c r="B126" t="n" s="56">
+      <c r="B126" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="C126" t="s" s="55">
+      <c r="C126" t="s" s="103">
         <v>15</v>
       </c>
-      <c r="D126" t="n" s="56">
+      <c r="D126" t="n" s="104">
         <v>160.0</v>
       </c>
-      <c r="E126" t="s" s="55">
+      <c r="E126" t="s" s="103">
         <v>16</v>
       </c>
-      <c r="F126" t="n" s="60">
-        <v>417.0</v>
+      <c r="F126" t="n" s="108">
+        <v>397.0</v>
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="s" s="55">
+      <c r="A127" t="s" s="103">
         <v>17</v>
       </c>
-      <c r="B127" t="n" s="56">
-        <v>3.555601966640625E9</v>
-      </c>
-      <c r="C127" t="s" s="55">
+      <c r="B127" t="n" s="104">
+        <v>3.1029216077539062E9</v>
+      </c>
+      <c r="C127" t="s" s="103">
         <v>18</v>
       </c>
-      <c r="D127" t="n" s="56">
+      <c r="D127" t="n" s="104">
         <v>9999999.0</v>
       </c>
-      <c r="E127" t="s" s="55">
+      <c r="E127" t="s" s="103">
         <v>19</v>
       </c>
-      <c r="F127" t="n" s="59">
-        <v>355.5601806640625</v>
+      <c r="F127" t="n" s="107">
+        <v>310.2921447753906</v>
       </c>
     </row>
     <row r="128"/>
@@ -18749,19 +18949,19 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>19.0</v>
+        <v>45.0</v>
       </c>
       <c r="B131" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="C131" t="n">
-        <v>31.906112670898438</v>
+        <v>31.320919036865234</v>
       </c>
       <c r="D131" t="n">
-        <v>264.5569058120526</v>
+        <v>196.6523324938246</v>
       </c>
       <c r="E131" t="n">
-        <v>18.384777069091797</v>
+        <v>40.26164245605469</v>
       </c>
       <c r="F131" t="n">
         <v>1.0</v>
@@ -18769,19 +18969,19 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>42.0</v>
+        <v>15.0</v>
       </c>
       <c r="B132" t="n">
-        <v>13.0</v>
+        <v>10.0</v>
       </c>
       <c r="C132" t="n">
-        <v>31.320919036865234</v>
+        <v>24.73863410949707</v>
       </c>
       <c r="D132" t="n">
-        <v>152.0144894752111</v>
+        <v>350.81816695114793</v>
       </c>
       <c r="E132" t="n">
-        <v>8.5440034866333</v>
+        <v>6.7082037925720215</v>
       </c>
       <c r="F132" t="n">
         <v>1.0</v>
@@ -18789,19 +18989,19 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>17.0</v>
+        <v>5.0</v>
       </c>
       <c r="B133" t="n">
-        <v>3.0</v>
+        <v>21.0</v>
       </c>
       <c r="C133" t="n">
-        <v>17.262676239013672</v>
+        <v>14.142135620117188</v>
       </c>
       <c r="D133" t="n">
-        <v>164.42302223578986</v>
+        <v>360.0</v>
       </c>
       <c r="E133" t="n">
-        <v>14.317821502685547</v>
+        <v>14.560219764709473</v>
       </c>
       <c r="F133" t="n">
         <v>1.0</v>
@@ -18809,19 +19009,19 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>45.0</v>
+        <v>49.0</v>
       </c>
       <c r="B134" t="n">
-        <v>10.0</v>
+        <v>18.0</v>
       </c>
       <c r="C134" t="n">
-        <v>31.320919036865234</v>
+        <v>21.63330841064453</v>
       </c>
       <c r="D134" t="n">
-        <v>196.6523324938246</v>
+        <v>304.9704733621193</v>
       </c>
       <c r="E134" t="n">
-        <v>17.69180679321289</v>
+        <v>8.246211051940918</v>
       </c>
       <c r="F134" t="n">
         <v>1.0</v>
@@ -18829,19 +19029,19 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>33.0</v>
+        <v>10.0</v>
       </c>
       <c r="B135" t="n">
-        <v>23.0</v>
+        <v>5.0</v>
       </c>
       <c r="C135" t="n">
-        <v>34.0</v>
+        <v>28.319604873657227</v>
       </c>
       <c r="D135" t="n">
-        <v>157.54908042266146</v>
+        <v>238.80064659365183</v>
       </c>
       <c r="E135" t="n">
-        <v>7.0</v>
+        <v>7.6157732009887695</v>
       </c>
       <c r="F135" t="n">
         <v>1.0</v>
@@ -18849,19 +19049,19 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>10.0</v>
+        <v>30.0</v>
       </c>
       <c r="B136" t="n">
-        <v>5.0</v>
+        <v>19.0</v>
       </c>
       <c r="C136" t="n">
-        <v>28.319604873657227</v>
+        <v>30.870698928833008</v>
       </c>
       <c r="D136" t="n">
-        <v>238.80064659365183</v>
+        <v>187.07804971242513</v>
       </c>
       <c r="E136" t="n">
-        <v>12.083045959472656</v>
+        <v>9.219544410705566</v>
       </c>
       <c r="F136" t="n">
         <v>1.0</v>
@@ -18869,19 +19069,19 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>34.0</v>
+        <v>9.0</v>
       </c>
       <c r="B137" t="n">
-        <v>26.0</v>
+        <v>11.0</v>
       </c>
       <c r="C137" t="n">
-        <v>31.78049659729004</v>
+        <v>23.0867919921875</v>
       </c>
       <c r="D137" t="n">
-        <v>338.16739400253954</v>
+        <v>171.05352046358252</v>
       </c>
       <c r="E137" t="n">
-        <v>15.620499610900879</v>
+        <v>8.485280990600586</v>
       </c>
       <c r="F137" t="n">
         <v>1.0</v>
@@ -18901,7 +19101,7 @@
         <v>345.5992243656941</v>
       </c>
       <c r="E138" t="n">
-        <v>6.4031243324279785</v>
+        <v>5.656854152679443</v>
       </c>
       <c r="F138" t="n">
         <v>1.0</v>
@@ -18909,19 +19109,19 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>21.0</v>
+        <v>34.0</v>
       </c>
       <c r="B139" t="n">
-        <v>8.0</v>
+        <v>26.0</v>
       </c>
       <c r="C139" t="n">
-        <v>32.06243896484375</v>
+        <v>31.78049659729004</v>
       </c>
       <c r="D139" t="n">
-        <v>359.656656935923</v>
+        <v>338.16739400253954</v>
       </c>
       <c r="E139" t="n">
-        <v>7.8102498054504395</v>
+        <v>6.4031243324279785</v>
       </c>
       <c r="F139" t="n">
         <v>1.0</v>
@@ -18929,19 +19129,19 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>29.0</v>
+        <v>21.0</v>
       </c>
       <c r="B140" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="C140" t="n">
-        <v>29.120439529418945</v>
+        <v>32.06243896484375</v>
       </c>
       <c r="D140" t="n">
-        <v>187.07804971242513</v>
+        <v>359.656656935923</v>
       </c>
       <c r="E140" t="n">
-        <v>7.211102485656738</v>
+        <v>9.05538558959961</v>
       </c>
       <c r="F140" t="n">
         <v>1.0</v>
@@ -18949,19 +19149,19 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>16.0</v>
+        <v>29.0</v>
       </c>
       <c r="B141" t="n">
-        <v>15.0</v>
+        <v>6.0</v>
       </c>
       <c r="C141" t="n">
-        <v>22.022714614868164</v>
+        <v>29.120439529418945</v>
       </c>
       <c r="D141" t="n">
-        <v>171.05352046358252</v>
+        <v>187.07804971242513</v>
       </c>
       <c r="E141" t="n">
-        <v>9.219544410705566</v>
+        <v>7.211102485656738</v>
       </c>
       <c r="F141" t="n">
         <v>1.0</v>
@@ -18969,19 +19169,19 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>11.0</v>
+        <v>16.0</v>
       </c>
       <c r="B142" t="n">
-        <v>19.0</v>
+        <v>15.0</v>
       </c>
       <c r="C142" t="n">
-        <v>12.041594505310059</v>
+        <v>22.022714614868164</v>
       </c>
       <c r="D142" t="n">
-        <v>323.25993313398806</v>
+        <v>171.05352046358252</v>
       </c>
       <c r="E142" t="n">
-        <v>10.0</v>
+        <v>9.219544410705566</v>
       </c>
       <c r="F142" t="n">
         <v>1.0</v>
@@ -18989,19 +19189,19 @@
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>35.0</v>
+        <v>2.0</v>
       </c>
       <c r="B143" t="n">
-        <v>17.0</v>
+        <v>30.0</v>
       </c>
       <c r="C143" t="n">
-        <v>39.408119201660156</v>
+        <v>21.02379608154297</v>
       </c>
       <c r="D143" t="n">
-        <v>359.656656935923</v>
+        <v>8.387652948531183</v>
       </c>
       <c r="E143" t="n">
-        <v>29.73213768005371</v>
+        <v>8.5440034866333</v>
       </c>
       <c r="F143" t="n">
         <v>1.0</v>
@@ -19009,19 +19209,19 @@
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>28.0</v>
+        <v>35.0</v>
       </c>
       <c r="B144" t="n">
-        <v>14.0</v>
+        <v>17.0</v>
       </c>
       <c r="C144" t="n">
-        <v>29.96664810180664</v>
+        <v>39.408119201660156</v>
       </c>
       <c r="D144" t="n">
-        <v>4.644742023417905</v>
+        <v>359.656656935923</v>
       </c>
       <c r="E144" t="n">
-        <v>19.416488647460938</v>
+        <v>19.10497283935547</v>
       </c>
       <c r="F144" t="n">
         <v>1.0</v>
@@ -19029,19 +19229,19 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>31.0</v>
+        <v>3.0</v>
       </c>
       <c r="B145" t="n">
-        <v>11.0</v>
+        <v>16.0</v>
       </c>
       <c r="C145" t="n">
-        <v>29.832868576049805</v>
+        <v>32.557640075683594</v>
       </c>
       <c r="D145" t="n">
-        <v>353.7970010977599</v>
+        <v>171.05352046358252</v>
       </c>
       <c r="E145" t="n">
-        <v>6.324555397033691</v>
+        <v>10.049875259399414</v>
       </c>
       <c r="F145" t="n">
         <v>1.0</v>
@@ -19049,19 +19249,19 @@
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="B146" t="n">
-        <v>7.0</v>
+        <v>23.0</v>
       </c>
       <c r="C146" t="n">
-        <v>13.892443656921387</v>
+        <v>22.022714614868164</v>
       </c>
       <c r="D146" t="n">
-        <v>353.7970010977599</v>
+        <v>337.0548166268401</v>
       </c>
       <c r="E146" t="n">
-        <v>17.0</v>
+        <v>21.095022201538086</v>
       </c>
       <c r="F146" t="n">
         <v>1.0</v>
@@ -19069,19 +19269,19 @@
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
       <c r="B147" t="n">
-        <v>29.0</v>
+        <v>7.0</v>
       </c>
       <c r="C147" t="n">
-        <v>8.062257766723633</v>
+        <v>13.892443656921387</v>
       </c>
       <c r="D147" t="n">
-        <v>337.0548166268401</v>
+        <v>353.7970010977599</v>
       </c>
       <c r="E147" t="n">
-        <v>20.880613327026367</v>
+        <v>11.661903381347656</v>
       </c>
       <c r="F147" t="n">
         <v>1.0</v>
@@ -19089,19 +19289,19 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>47.0</v>
+        <v>27.0</v>
       </c>
       <c r="B148" t="n">
-        <v>25.0</v>
+        <v>15.0</v>
       </c>
       <c r="C148" t="n">
-        <v>9.433980941772461</v>
+        <v>8.0</v>
       </c>
       <c r="D148" t="n">
-        <v>315.2115326768105</v>
+        <v>6.338943043987854</v>
       </c>
       <c r="E148" t="n">
-        <v>6.0</v>
+        <v>8.062257766723633</v>
       </c>
       <c r="F148" t="n">
         <v>1.0</v>
@@ -19109,19 +19309,19 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>18.0</v>
+        <v>11.0</v>
       </c>
       <c r="B149" t="n">
-        <v>41.0</v>
+        <v>19.0</v>
       </c>
       <c r="C149" t="n">
-        <v>14.764822959899902</v>
+        <v>12.041594505310059</v>
       </c>
       <c r="D149" t="n">
-        <v>336.359591450648</v>
+        <v>323.25993313398806</v>
       </c>
       <c r="E149" t="n">
-        <v>8.062257766723633</v>
+        <v>13.892443656921387</v>
       </c>
       <c r="F149" t="n">
         <v>1.0</v>
@@ -19129,19 +19329,19 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>48.0</v>
+        <v>38.0</v>
       </c>
       <c r="B150" t="n">
-        <v>17.0</v>
+        <v>15.0</v>
       </c>
       <c r="C150" t="n">
         <v>15.81138801574707</v>
       </c>
       <c r="D150" t="n">
-        <v>315.2115326768105</v>
+        <v>216.59028435753538</v>
       </c>
       <c r="E150" t="n">
-        <v>23.409399032592773</v>
+        <v>6.7082037925720215</v>
       </c>
       <c r="F150" t="n">
         <v>1.0</v>
@@ -19149,19 +19349,19 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>23.0</v>
+        <v>37.0</v>
       </c>
       <c r="B151" t="n">
-        <v>16.0</v>
+        <v>9.0</v>
       </c>
       <c r="C151" t="n">
-        <v>22.022714614868164</v>
+        <v>18.11077117919922</v>
       </c>
       <c r="D151" t="n">
-        <v>299.7015117237478</v>
+        <v>251.4270412434094</v>
       </c>
       <c r="E151" t="n">
-        <v>9.219544410705566</v>
+        <v>18.384777069091797</v>
       </c>
       <c r="F151" t="n">
         <v>1.0</v>
@@ -19169,19 +19369,19 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>43.0</v>
+        <v>17.0</v>
       </c>
       <c r="B152" t="n">
-        <v>11.0</v>
+        <v>3.0</v>
       </c>
       <c r="C152" t="n">
-        <v>34.65544509887695</v>
+        <v>17.262676239013672</v>
       </c>
       <c r="D152" t="n">
-        <v>8.319952741629265</v>
+        <v>164.42302223578986</v>
       </c>
       <c r="E152" t="n">
-        <v>13.03840446472168</v>
+        <v>5.099019527435303</v>
       </c>
       <c r="F152" t="n">
         <v>1.0</v>
@@ -19189,19 +19389,19 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>24.0</v>
+        <v>18.0</v>
       </c>
       <c r="B153" t="n">
-        <v>10.0</v>
+        <v>41.0</v>
       </c>
       <c r="C153" t="n">
-        <v>25.05992889404297</v>
+        <v>14.764822959899902</v>
       </c>
       <c r="D153" t="n">
-        <v>171.97940109631875</v>
+        <v>336.359591450648</v>
       </c>
       <c r="E153" t="n">
-        <v>12.369317054748535</v>
+        <v>14.142135620117188</v>
       </c>
       <c r="F153" t="n">
         <v>1.0</v>
@@ -19209,19 +19409,19 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
       </c>
       <c r="B154" t="n">
-        <v>21.0</v>
+        <v>27.0</v>
       </c>
       <c r="C154" t="n">
-        <v>18.11077117919922</v>
+        <v>30.479501724243164</v>
       </c>
       <c r="D154" t="n">
-        <v>346.6473834054614</v>
+        <v>298.9856443268601</v>
       </c>
       <c r="E154" t="n">
-        <v>10.770329475402832</v>
+        <v>17.464248657226562</v>
       </c>
       <c r="F154" t="n">
         <v>1.0</v>
@@ -19229,19 +19429,19 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>25.0</v>
+        <v>19.0</v>
       </c>
       <c r="B155" t="n">
-        <v>28.0</v>
+        <v>9.0</v>
       </c>
       <c r="C155" t="n">
-        <v>23.0867919921875</v>
+        <v>31.906112670898438</v>
       </c>
       <c r="D155" t="n">
-        <v>240.25810175410237</v>
+        <v>264.5569058120526</v>
       </c>
       <c r="E155" t="n">
-        <v>6.4031243324279785</v>
+        <v>5.0</v>
       </c>
       <c r="F155" t="n">
         <v>1.0</v>
@@ -19249,19 +19449,19 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>13.0</v>
+        <v>40.0</v>
       </c>
       <c r="B156" t="n">
-        <v>23.0</v>
+        <v>7.0</v>
       </c>
       <c r="C156" t="n">
-        <v>29.154760360717773</v>
+        <v>42.20189666748047</v>
       </c>
       <c r="D156" t="n">
         <v>8.319952741629265</v>
       </c>
       <c r="E156" t="n">
-        <v>13.152946472167969</v>
+        <v>10.630146026611328</v>
       </c>
       <c r="F156" t="n">
         <v>1.0</v>
@@ -19281,94 +19481,94 @@
         <v>303.7008314149076</v>
       </c>
       <c r="E157" t="n">
-        <v>25.495098114013672</v>
+        <v>7.8102498054504395</v>
       </c>
       <c r="F157" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="158">
-      <c r="A158" t="s" s="55">
+      <c r="A158" t="s" s="103">
         <v>27</v>
       </c>
-      <c r="B158" s="59" t="n">
+      <c r="B158" s="107" t="n">
         <f>SUM(B130:B157)</f>
-        <v>417.0</v>
-      </c>
-      <c r="E158" s="59" t="n">
+        <v>397.0</v>
+      </c>
+      <c r="E158" s="107" t="n">
         <f>SUM(E130:E157)</f>
-        <v>355.56019163131714</v>
+        <v>310.29214572906494</v>
       </c>
     </row>
     <row r="159"/>
     <row r="160"/>
     <row r="161"/>
     <row r="162">
-      <c r="A162" t="s" s="55">
+      <c r="A162" t="s" s="103">
         <v>10</v>
       </c>
-      <c r="B162" t="n" s="56">
+      <c r="B162" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="C162" t="s" s="55">
+      <c r="C162" t="s" s="103">
         <v>11</v>
       </c>
-      <c r="D162" t="n" s="56">
+      <c r="D162" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="E162" t="s" s="55">
+      <c r="E162" t="s" s="103">
         <v>12</v>
       </c>
-      <c r="F162" t="n" s="56">
+      <c r="F162" t="n" s="104">
         <v>-1.0</v>
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="s" s="55">
+      <c r="A163" t="s" s="103">
         <v>13</v>
       </c>
-      <c r="B163" t="n" s="56">
+      <c r="B163" t="n" s="104">
         <v>0.0</v>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="s" s="55">
+      <c r="A164" t="s" s="103">
         <v>14</v>
       </c>
-      <c r="B164" t="n" s="56">
+      <c r="B164" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="C164" t="s" s="55">
+      <c r="C164" t="s" s="103">
         <v>15</v>
       </c>
-      <c r="D164" t="n" s="56">
+      <c r="D164" t="n" s="104">
         <v>160.0</v>
       </c>
-      <c r="E164" t="s" s="55">
+      <c r="E164" t="s" s="103">
         <v>16</v>
       </c>
-      <c r="F164" t="n" s="60">
-        <v>520.0</v>
+      <c r="F164" t="n" s="108">
+        <v>540.0</v>
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="s" s="55">
+      <c r="A165" t="s" s="103">
         <v>17</v>
       </c>
-      <c r="B165" t="n" s="56">
-        <v>3.0180735852929688E9</v>
-      </c>
-      <c r="C165" t="s" s="55">
+      <c r="B165" t="n" s="104">
+        <v>3.6276982190820312E9</v>
+      </c>
+      <c r="C165" t="s" s="103">
         <v>18</v>
       </c>
-      <c r="D165" t="n" s="56">
+      <c r="D165" t="n" s="104">
         <v>9999999.0</v>
       </c>
-      <c r="E165" t="s" s="55">
+      <c r="E165" t="s" s="103">
         <v>19</v>
       </c>
-      <c r="F165" t="n" s="59">
-        <v>301.8073425292969</v>
+      <c r="F165" t="n" s="107">
+        <v>362.7698059082031</v>
       </c>
     </row>
     <row r="166"/>
@@ -19414,19 +19614,19 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>40.0</v>
+        <v>13.0</v>
       </c>
       <c r="B169" t="n">
-        <v>7.0</v>
+        <v>23.0</v>
       </c>
       <c r="C169" t="n">
-        <v>42.20189666748047</v>
+        <v>29.154760360717773</v>
       </c>
       <c r="D169" t="n">
         <v>8.319952741629265</v>
       </c>
       <c r="E169" t="n">
-        <v>7.8102498054504395</v>
+        <v>25.495098114013672</v>
       </c>
       <c r="F169" t="n">
         <v>1.0</v>
@@ -19434,19 +19634,19 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>41.0</v>
+        <v>25.0</v>
       </c>
       <c r="B170" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="C170" t="n">
-        <v>30.479501724243164</v>
+        <v>23.0867919921875</v>
       </c>
       <c r="D170" t="n">
-        <v>298.9856443268601</v>
+        <v>240.25810175410237</v>
       </c>
       <c r="E170" t="n">
-        <v>12.083045959472656</v>
+        <v>13.152946472167969</v>
       </c>
       <c r="F170" t="n">
         <v>1.0</v>
@@ -19454,19 +19654,19 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>4.0</v>
+        <v>14.0</v>
       </c>
       <c r="B171" t="n">
-        <v>9.0</v>
+        <v>21.0</v>
       </c>
       <c r="C171" t="n">
-        <v>17.20465087890625</v>
+        <v>18.11077117919922</v>
       </c>
       <c r="D171" t="n">
-        <v>206.94372235198546</v>
+        <v>346.6473834054614</v>
       </c>
       <c r="E171" t="n">
-        <v>13.45362377166748</v>
+        <v>6.4031243324279785</v>
       </c>
       <c r="F171" t="n">
         <v>1.0</v>
@@ -19474,19 +19674,19 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>51.0</v>
+        <v>24.0</v>
       </c>
       <c r="B172" t="n">
-        <v>160.0</v>
+        <v>10.0</v>
       </c>
       <c r="C172" t="n">
-        <v>0.0</v>
+        <v>25.05992889404297</v>
       </c>
       <c r="D172" t="n">
-        <v>6.338943043987854</v>
+        <v>171.97940109631875</v>
       </c>
       <c r="E172" t="n">
-        <v>17.20465087890625</v>
+        <v>10.770329475402832</v>
       </c>
       <c r="F172" t="n">
         <v>1.0</v>
@@ -19494,19 +19694,19 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>46.0</v>
+        <v>43.0</v>
       </c>
       <c r="B173" t="n">
-        <v>5.0</v>
+        <v>11.0</v>
       </c>
       <c r="C173" t="n">
-        <v>2.2360680103302</v>
+        <v>34.65544509887695</v>
       </c>
       <c r="D173" t="n">
-        <v>251.4270412434094</v>
+        <v>8.319952741629265</v>
       </c>
       <c r="E173" t="n">
-        <v>2.2360680103302</v>
+        <v>12.369317054748535</v>
       </c>
       <c r="F173" t="n">
         <v>1.0</v>
@@ -19514,19 +19714,19 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>32.0</v>
+        <v>23.0</v>
       </c>
       <c r="B174" t="n">
-        <v>12.0</v>
+        <v>16.0</v>
       </c>
       <c r="C174" t="n">
-        <v>10.0</v>
+        <v>22.022714614868164</v>
       </c>
       <c r="D174" t="n">
-        <v>276.470003989416</v>
+        <v>299.7015117237478</v>
       </c>
       <c r="E174" t="n">
-        <v>9.219544410705566</v>
+        <v>13.03840446472168</v>
       </c>
       <c r="F174" t="n">
         <v>1.0</v>
@@ -19534,19 +19734,19 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>27.0</v>
+        <v>7.0</v>
       </c>
       <c r="B175" t="n">
-        <v>15.0</v>
+        <v>19.0</v>
       </c>
       <c r="C175" t="n">
-        <v>8.0</v>
+        <v>26.419689178466797</v>
       </c>
       <c r="D175" t="n">
-        <v>6.338943043987854</v>
+        <v>336.359591450648</v>
       </c>
       <c r="E175" t="n">
-        <v>8.246211051940918</v>
+        <v>6.082762718200684</v>
       </c>
       <c r="F175" t="n">
         <v>1.0</v>
@@ -19554,19 +19754,19 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>6.0</v>
+        <v>26.0</v>
       </c>
       <c r="B176" t="n">
-        <v>15.0</v>
+        <v>7.0</v>
       </c>
       <c r="C176" t="n">
-        <v>11.401754379272461</v>
+        <v>28.160255432128906</v>
       </c>
       <c r="D176" t="n">
-        <v>152.0144894752111</v>
+        <v>164.42302223578986</v>
       </c>
       <c r="E176" t="n">
-        <v>9.05538558959961</v>
+        <v>11.180339813232422</v>
       </c>
       <c r="F176" t="n">
         <v>1.0</v>
@@ -19574,19 +19774,19 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>7.0</v>
+        <v>48.0</v>
       </c>
       <c r="B177" t="n">
-        <v>19.0</v>
+        <v>17.0</v>
       </c>
       <c r="C177" t="n">
-        <v>26.419689178466797</v>
+        <v>15.81138801574707</v>
       </c>
       <c r="D177" t="n">
-        <v>336.359591450648</v>
+        <v>315.2115326768105</v>
       </c>
       <c r="E177" t="n">
-        <v>16.492422103881836</v>
+        <v>13.152946472167969</v>
       </c>
       <c r="F177" t="n">
         <v>1.0</v>
@@ -19594,19 +19794,19 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>26.0</v>
+        <v>6.0</v>
       </c>
       <c r="B178" t="n">
-        <v>7.0</v>
+        <v>15.0</v>
       </c>
       <c r="C178" t="n">
-        <v>28.160255432128906</v>
+        <v>11.401754379272461</v>
       </c>
       <c r="D178" t="n">
-        <v>164.42302223578986</v>
+        <v>152.0144894752111</v>
       </c>
       <c r="E178" t="n">
-        <v>11.180339813232422</v>
+        <v>8.9442720413208</v>
       </c>
       <c r="F178" t="n">
         <v>1.0</v>
@@ -19614,19 +19814,19 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B179" t="n">
         <v>8.0</v>
       </c>
-      <c r="B179" t="n">
-        <v>23.0</v>
-      </c>
       <c r="C179" t="n">
-        <v>22.022714614868164</v>
+        <v>20.808652877807617</v>
       </c>
       <c r="D179" t="n">
-        <v>337.0548166268401</v>
+        <v>323.25993313398806</v>
       </c>
       <c r="E179" t="n">
-        <v>7.211102485656738</v>
+        <v>23.25940704345703</v>
       </c>
       <c r="F179" t="n">
         <v>1.0</v>
@@ -19634,19 +19834,19 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>22.0</v>
+        <v>31.0</v>
       </c>
       <c r="B180" t="n">
-        <v>8.0</v>
+        <v>11.0</v>
       </c>
       <c r="C180" t="n">
-        <v>20.808652877807617</v>
+        <v>29.832868576049805</v>
       </c>
       <c r="D180" t="n">
-        <v>323.25993313398806</v>
+        <v>353.7970010977599</v>
       </c>
       <c r="E180" t="n">
-        <v>12.083045959472656</v>
+        <v>13.0</v>
       </c>
       <c r="F180" t="n">
         <v>1.0</v>
@@ -19654,19 +19854,19 @@
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>3.0</v>
+        <v>28.0</v>
       </c>
       <c r="B181" t="n">
-        <v>16.0</v>
+        <v>14.0</v>
       </c>
       <c r="C181" t="n">
-        <v>32.557640075683594</v>
+        <v>29.96664810180664</v>
       </c>
       <c r="D181" t="n">
-        <v>171.05352046358252</v>
+        <v>4.644742023417905</v>
       </c>
       <c r="E181" t="n">
-        <v>12.206555366516113</v>
+        <v>6.324555397033691</v>
       </c>
       <c r="F181" t="n">
         <v>1.0</v>
@@ -19686,7 +19886,7 @@
         <v>288.540600851905</v>
       </c>
       <c r="E182" t="n">
-        <v>12.083045959472656</v>
+        <v>20.099750518798828</v>
       </c>
       <c r="F182" t="n">
         <v>1.0</v>
@@ -19714,19 +19914,19 @@
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>2.0</v>
+        <v>32.0</v>
       </c>
       <c r="B184" t="n">
-        <v>30.0</v>
+        <v>12.0</v>
       </c>
       <c r="C184" t="n">
-        <v>21.02379608154297</v>
+        <v>10.0</v>
       </c>
       <c r="D184" t="n">
-        <v>8.387652948531183</v>
+        <v>276.470003989416</v>
       </c>
       <c r="E184" t="n">
-        <v>12.041594505310059</v>
+        <v>22.472204208374023</v>
       </c>
       <c r="F184" t="n">
         <v>1.0</v>
@@ -19734,19 +19934,19 @@
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>9.0</v>
+        <v>46.0</v>
       </c>
       <c r="B185" t="n">
-        <v>11.0</v>
+        <v>5.0</v>
       </c>
       <c r="C185" t="n">
-        <v>23.0867919921875</v>
+        <v>2.2360680103302</v>
       </c>
       <c r="D185" t="n">
-        <v>171.05352046358252</v>
+        <v>251.4270412434094</v>
       </c>
       <c r="E185" t="n">
-        <v>16.278820037841797</v>
+        <v>9.219544410705566</v>
       </c>
       <c r="F185" t="n">
         <v>1.0</v>
@@ -19754,19 +19954,19 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>30.0</v>
+        <v>51.0</v>
       </c>
       <c r="B186" t="n">
-        <v>19.0</v>
+        <v>160.0</v>
       </c>
       <c r="C186" t="n">
-        <v>30.870698928833008</v>
+        <v>0.0</v>
       </c>
       <c r="D186" t="n">
-        <v>187.07804971242513</v>
+        <v>6.338943043987854</v>
       </c>
       <c r="E186" t="n">
-        <v>8.485280990600586</v>
+        <v>2.2360680103302</v>
       </c>
       <c r="F186" t="n">
         <v>1.0</v>
@@ -19774,19 +19974,19 @@
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>39.0</v>
+        <v>47.0</v>
       </c>
       <c r="B187" t="n">
-        <v>14.0</v>
+        <v>25.0</v>
       </c>
       <c r="C187" t="n">
-        <v>38.28837966918945</v>
+        <v>9.433980941772461</v>
       </c>
       <c r="D187" t="n">
-        <v>321.1319132345335</v>
+        <v>315.2115326768105</v>
       </c>
       <c r="E187" t="n">
-        <v>12.041594505310059</v>
+        <v>9.433980941772461</v>
       </c>
       <c r="F187" t="n">
         <v>1.0</v>
@@ -19794,19 +19994,19 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>49.0</v>
+        <v>12.0</v>
       </c>
       <c r="B188" t="n">
-        <v>18.0</v>
+        <v>29.0</v>
       </c>
       <c r="C188" t="n">
-        <v>21.63330841064453</v>
+        <v>8.062257766723633</v>
       </c>
       <c r="D188" t="n">
-        <v>304.9704733621193</v>
+        <v>337.0548166268401</v>
       </c>
       <c r="E188" t="n">
-        <v>17.029386520385742</v>
+        <v>6.0</v>
       </c>
       <c r="F188" t="n">
         <v>1.0</v>
@@ -19814,19 +20014,19 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>38.0</v>
+        <v>39.0</v>
       </c>
       <c r="B189" t="n">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="C189" t="n">
-        <v>15.81138801574707</v>
+        <v>38.28837966918945</v>
       </c>
       <c r="D189" t="n">
-        <v>216.59028435753538</v>
+        <v>321.1319132345335</v>
       </c>
       <c r="E189" t="n">
-        <v>7.6157732009887695</v>
+        <v>32.75667953491211</v>
       </c>
       <c r="F189" t="n">
         <v>1.0</v>
@@ -19834,19 +20034,19 @@
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>5.0</v>
+        <v>33.0</v>
       </c>
       <c r="B190" t="n">
-        <v>21.0</v>
+        <v>23.0</v>
       </c>
       <c r="C190" t="n">
-        <v>14.142135620117188</v>
+        <v>34.0</v>
       </c>
       <c r="D190" t="n">
-        <v>360.0</v>
+        <v>157.54908042266146</v>
       </c>
       <c r="E190" t="n">
-        <v>7.071067810058594</v>
+        <v>13.928388595581055</v>
       </c>
       <c r="F190" t="n">
         <v>1.0</v>
@@ -19854,19 +20054,19 @@
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>37.0</v>
+        <v>44.0</v>
       </c>
       <c r="B191" t="n">
-        <v>9.0</v>
+        <v>16.0</v>
       </c>
       <c r="C191" t="n">
-        <v>18.11077117919922</v>
+        <v>25.0</v>
       </c>
       <c r="D191" t="n">
-        <v>251.4270412434094</v>
+        <v>6.338943043987854</v>
       </c>
       <c r="E191" t="n">
-        <v>11.313708305358887</v>
+        <v>16.76305389404297</v>
       </c>
       <c r="F191" t="n">
         <v>1.0</v>
@@ -19874,19 +20074,19 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>15.0</v>
+        <v>4.0</v>
       </c>
       <c r="B192" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="C192" t="n">
-        <v>24.73863410949707</v>
+        <v>17.20465087890625</v>
       </c>
       <c r="D192" t="n">
-        <v>350.81816695114793</v>
+        <v>206.94372235198546</v>
       </c>
       <c r="E192" t="n">
-        <v>7.211102485656738</v>
+        <v>14.866068840026855</v>
       </c>
       <c r="F192" t="n">
         <v>1.0</v>
@@ -19894,19 +20094,19 @@
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>44.0</v>
+        <v>42.0</v>
       </c>
       <c r="B193" t="n">
-        <v>16.0</v>
+        <v>13.0</v>
       </c>
       <c r="C193" t="n">
-        <v>25.0</v>
+        <v>31.320919036865234</v>
       </c>
       <c r="D193" t="n">
-        <v>6.338943043987854</v>
+        <v>152.0144894752111</v>
       </c>
       <c r="E193" t="n">
-        <v>6.082762718200684</v>
+        <v>16.031219482421875</v>
       </c>
       <c r="F193" t="n">
         <v>1.0</v>
@@ -19926,94 +20126,94 @@
         <v>303.7008314149076</v>
       </c>
       <c r="E194" t="n">
-        <v>33.541019439697266</v>
+        <v>23.25940704345703</v>
       </c>
       <c r="F194" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="195">
-      <c r="A195" t="s" s="55">
+      <c r="A195" t="s" s="103">
         <v>27</v>
       </c>
-      <c r="B195" s="59" t="n">
+      <c r="B195" s="107" t="n">
         <f>SUM(B168:B194)</f>
-        <v>520.0</v>
-      </c>
-      <c r="E195" s="59" t="n">
+        <v>540.0</v>
+      </c>
+      <c r="E195" s="107" t="n">
         <f>SUM(E168:E194)</f>
-        <v>301.8073661327362</v>
+        <v>362.7698333263397</v>
       </c>
     </row>
     <row r="196"/>
     <row r="197"/>
     <row r="198"/>
     <row r="199">
-      <c r="A199" t="s" s="55">
+      <c r="A199" t="s" s="103">
         <v>10</v>
       </c>
-      <c r="B199" t="n" s="56">
+      <c r="B199" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="C199" t="s" s="55">
+      <c r="C199" t="s" s="103">
         <v>11</v>
       </c>
-      <c r="D199" t="n" s="56">
+      <c r="D199" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="E199" t="s" s="55">
+      <c r="E199" t="s" s="103">
         <v>12</v>
       </c>
-      <c r="F199" t="n" s="56">
+      <c r="F199" t="n" s="104">
         <v>-1.0</v>
       </c>
     </row>
     <row r="200">
-      <c r="A200" t="s" s="55">
+      <c r="A200" t="s" s="103">
         <v>13</v>
       </c>
-      <c r="B200" t="n" s="56">
+      <c r="B200" t="n" s="104">
         <v>1.0</v>
       </c>
     </row>
     <row r="201">
-      <c r="A201" t="s" s="55">
+      <c r="A201" t="s" s="103">
         <v>14</v>
       </c>
-      <c r="B201" t="n" s="56">
+      <c r="B201" t="n" s="104">
         <v>-1.0</v>
       </c>
-      <c r="C201" t="s" s="55">
+      <c r="C201" t="s" s="103">
         <v>15</v>
       </c>
-      <c r="D201" t="n" s="56">
+      <c r="D201" t="n" s="104">
         <v>160.0</v>
       </c>
-      <c r="E201" t="s" s="55">
+      <c r="E201" t="s" s="103">
         <v>16</v>
       </c>
-      <c r="F201" t="n" s="60">
-        <v>417.0</v>
+      <c r="F201" t="n" s="108">
+        <v>397.0</v>
       </c>
     </row>
     <row r="202">
-      <c r="A202" t="s" s="55">
+      <c r="A202" t="s" s="103">
         <v>17</v>
       </c>
-      <c r="B202" t="n" s="56">
-        <v>3.555601966640625E9</v>
-      </c>
-      <c r="C202" t="s" s="55">
+      <c r="B202" t="n" s="104">
+        <v>3.1029216077539062E9</v>
+      </c>
+      <c r="C202" t="s" s="103">
         <v>18</v>
       </c>
-      <c r="D202" t="n" s="56">
+      <c r="D202" t="n" s="104">
         <v>9999999.0</v>
       </c>
-      <c r="E202" t="s" s="55">
+      <c r="E202" t="s" s="103">
         <v>19</v>
       </c>
-      <c r="F202" t="n" s="59">
-        <v>355.5601806640625</v>
+      <c r="F202" t="n" s="107">
+        <v>310.2921447753906</v>
       </c>
     </row>
     <row r="203"/>
@@ -20059,19 +20259,19 @@
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>19.0</v>
+        <v>45.0</v>
       </c>
       <c r="B206" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="C206" t="n">
-        <v>31.906112670898438</v>
+        <v>31.320919036865234</v>
       </c>
       <c r="D206" t="n">
-        <v>264.5569058120526</v>
+        <v>196.6523324938246</v>
       </c>
       <c r="E206" t="n">
-        <v>18.384777069091797</v>
+        <v>40.26164245605469</v>
       </c>
       <c r="F206" t="n">
         <v>1.0</v>
@@ -20079,19 +20279,19 @@
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>42.0</v>
+        <v>15.0</v>
       </c>
       <c r="B207" t="n">
-        <v>13.0</v>
+        <v>10.0</v>
       </c>
       <c r="C207" t="n">
-        <v>31.320919036865234</v>
+        <v>24.73863410949707</v>
       </c>
       <c r="D207" t="n">
-        <v>152.0144894752111</v>
+        <v>350.81816695114793</v>
       </c>
       <c r="E207" t="n">
-        <v>8.5440034866333</v>
+        <v>6.7082037925720215</v>
       </c>
       <c r="F207" t="n">
         <v>1.0</v>
@@ -20099,19 +20299,19 @@
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>17.0</v>
+        <v>5.0</v>
       </c>
       <c r="B208" t="n">
-        <v>3.0</v>
+        <v>21.0</v>
       </c>
       <c r="C208" t="n">
-        <v>17.262676239013672</v>
+        <v>14.142135620117188</v>
       </c>
       <c r="D208" t="n">
-        <v>164.42302223578986</v>
+        <v>360.0</v>
       </c>
       <c r="E208" t="n">
-        <v>14.317821502685547</v>
+        <v>14.560219764709473</v>
       </c>
       <c r="F208" t="n">
         <v>1.0</v>
@@ -20119,19 +20319,19 @@
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>45.0</v>
+        <v>49.0</v>
       </c>
       <c r="B209" t="n">
-        <v>10.0</v>
+        <v>18.0</v>
       </c>
       <c r="C209" t="n">
-        <v>31.320919036865234</v>
+        <v>21.63330841064453</v>
       </c>
       <c r="D209" t="n">
-        <v>196.6523324938246</v>
+        <v>304.9704733621193</v>
       </c>
       <c r="E209" t="n">
-        <v>17.69180679321289</v>
+        <v>8.246211051940918</v>
       </c>
       <c r="F209" t="n">
         <v>1.0</v>
@@ -20139,19 +20339,19 @@
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>33.0</v>
+        <v>10.0</v>
       </c>
       <c r="B210" t="n">
-        <v>23.0</v>
+        <v>5.0</v>
       </c>
       <c r="C210" t="n">
-        <v>34.0</v>
+        <v>28.319604873657227</v>
       </c>
       <c r="D210" t="n">
-        <v>157.54908042266146</v>
+        <v>238.80064659365183</v>
       </c>
       <c r="E210" t="n">
-        <v>7.0</v>
+        <v>7.6157732009887695</v>
       </c>
       <c r="F210" t="n">
         <v>1.0</v>
@@ -20159,19 +20359,19 @@
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>10.0</v>
+        <v>30.0</v>
       </c>
       <c r="B211" t="n">
-        <v>5.0</v>
+        <v>19.0</v>
       </c>
       <c r="C211" t="n">
-        <v>28.319604873657227</v>
+        <v>30.870698928833008</v>
       </c>
       <c r="D211" t="n">
-        <v>238.80064659365183</v>
+        <v>187.07804971242513</v>
       </c>
       <c r="E211" t="n">
-        <v>12.083045959472656</v>
+        <v>9.219544410705566</v>
       </c>
       <c r="F211" t="n">
         <v>1.0</v>
@@ -20179,19 +20379,19 @@
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>34.0</v>
+        <v>9.0</v>
       </c>
       <c r="B212" t="n">
-        <v>26.0</v>
+        <v>11.0</v>
       </c>
       <c r="C212" t="n">
-        <v>31.78049659729004</v>
+        <v>23.0867919921875</v>
       </c>
       <c r="D212" t="n">
-        <v>338.16739400253954</v>
+        <v>171.05352046358252</v>
       </c>
       <c r="E212" t="n">
-        <v>15.620499610900879</v>
+        <v>8.485280990600586</v>
       </c>
       <c r="F212" t="n">
         <v>1.0</v>
@@ -20211,7 +20411,7 @@
         <v>345.5992243656941</v>
       </c>
       <c r="E213" t="n">
-        <v>6.4031243324279785</v>
+        <v>5.656854152679443</v>
       </c>
       <c r="F213" t="n">
         <v>1.0</v>
@@ -20219,19 +20419,19 @@
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>21.0</v>
+        <v>34.0</v>
       </c>
       <c r="B214" t="n">
-        <v>8.0</v>
+        <v>26.0</v>
       </c>
       <c r="C214" t="n">
-        <v>32.06243896484375</v>
+        <v>31.78049659729004</v>
       </c>
       <c r="D214" t="n">
-        <v>359.656656935923</v>
+        <v>338.16739400253954</v>
       </c>
       <c r="E214" t="n">
-        <v>7.8102498054504395</v>
+        <v>6.4031243324279785</v>
       </c>
       <c r="F214" t="n">
         <v>1.0</v>
@@ -20239,19 +20439,19 @@
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>29.0</v>
+        <v>21.0</v>
       </c>
       <c r="B215" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="C215" t="n">
-        <v>29.120439529418945</v>
+        <v>32.06243896484375</v>
       </c>
       <c r="D215" t="n">
-        <v>187.07804971242513</v>
+        <v>359.656656935923</v>
       </c>
       <c r="E215" t="n">
-        <v>7.211102485656738</v>
+        <v>9.05538558959961</v>
       </c>
       <c r="F215" t="n">
         <v>1.0</v>
@@ -20259,19 +20459,19 @@
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>16.0</v>
+        <v>29.0</v>
       </c>
       <c r="B216" t="n">
-        <v>15.0</v>
+        <v>6.0</v>
       </c>
       <c r="C216" t="n">
-        <v>22.022714614868164</v>
+        <v>29.120439529418945</v>
       </c>
       <c r="D216" t="n">
-        <v>171.05352046358252</v>
+        <v>187.07804971242513</v>
       </c>
       <c r="E216" t="n">
-        <v>9.219544410705566</v>
+        <v>7.211102485656738</v>
       </c>
       <c r="F216" t="n">
         <v>1.0</v>
@@ -20279,19 +20479,19 @@
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>11.0</v>
+        <v>16.0</v>
       </c>
       <c r="B217" t="n">
-        <v>19.0</v>
+        <v>15.0</v>
       </c>
       <c r="C217" t="n">
-        <v>12.041594505310059</v>
+        <v>22.022714614868164</v>
       </c>
       <c r="D217" t="n">
-        <v>323.25993313398806</v>
+        <v>171.05352046358252</v>
       </c>
       <c r="E217" t="n">
-        <v>10.0</v>
+        <v>9.219544410705566</v>
       </c>
       <c r="F217" t="n">
         <v>1.0</v>
@@ -20299,19 +20499,19 @@
     </row>
     <row r="218">
       <c r="A218" t="n">
-        <v>35.0</v>
+        <v>2.0</v>
       </c>
       <c r="B218" t="n">
-        <v>17.0</v>
+        <v>30.0</v>
       </c>
       <c r="C218" t="n">
-        <v>39.408119201660156</v>
+        <v>21.02379608154297</v>
       </c>
       <c r="D218" t="n">
-        <v>359.656656935923</v>
+        <v>8.387652948531183</v>
       </c>
       <c r="E218" t="n">
-        <v>29.73213768005371</v>
+        <v>8.5440034866333</v>
       </c>
       <c r="F218" t="n">
         <v>1.0</v>
@@ -20319,19 +20519,19 @@
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>28.0</v>
+        <v>35.0</v>
       </c>
       <c r="B219" t="n">
-        <v>14.0</v>
+        <v>17.0</v>
       </c>
       <c r="C219" t="n">
-        <v>29.96664810180664</v>
+        <v>39.408119201660156</v>
       </c>
       <c r="D219" t="n">
-        <v>4.644742023417905</v>
+        <v>359.656656935923</v>
       </c>
       <c r="E219" t="n">
-        <v>19.416488647460938</v>
+        <v>19.10497283935547</v>
       </c>
       <c r="F219" t="n">
         <v>1.0</v>
@@ -20339,19 +20539,19 @@
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>31.0</v>
+        <v>3.0</v>
       </c>
       <c r="B220" t="n">
-        <v>11.0</v>
+        <v>16.0</v>
       </c>
       <c r="C220" t="n">
-        <v>29.832868576049805</v>
+        <v>32.557640075683594</v>
       </c>
       <c r="D220" t="n">
-        <v>353.7970010977599</v>
+        <v>171.05352046358252</v>
       </c>
       <c r="E220" t="n">
-        <v>6.324555397033691</v>
+        <v>10.049875259399414</v>
       </c>
       <c r="F220" t="n">
         <v>1.0</v>
@@ -20359,19 +20559,19 @@
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="B221" t="n">
-        <v>7.0</v>
+        <v>23.0</v>
       </c>
       <c r="C221" t="n">
-        <v>13.892443656921387</v>
+        <v>22.022714614868164</v>
       </c>
       <c r="D221" t="n">
-        <v>353.7970010977599</v>
+        <v>337.0548166268401</v>
       </c>
       <c r="E221" t="n">
-        <v>17.0</v>
+        <v>21.095022201538086</v>
       </c>
       <c r="F221" t="n">
         <v>1.0</v>
@@ -20379,19 +20579,19 @@
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
       <c r="B222" t="n">
-        <v>29.0</v>
+        <v>7.0</v>
       </c>
       <c r="C222" t="n">
-        <v>8.062257766723633</v>
+        <v>13.892443656921387</v>
       </c>
       <c r="D222" t="n">
-        <v>337.0548166268401</v>
+        <v>353.7970010977599</v>
       </c>
       <c r="E222" t="n">
-        <v>20.880613327026367</v>
+        <v>11.661903381347656</v>
       </c>
       <c r="F222" t="n">
         <v>1.0</v>
@@ -20399,19 +20599,19 @@
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>47.0</v>
+        <v>27.0</v>
       </c>
       <c r="B223" t="n">
-        <v>25.0</v>
+        <v>15.0</v>
       </c>
       <c r="C223" t="n">
-        <v>9.433980941772461</v>
+        <v>8.0</v>
       </c>
       <c r="D223" t="n">
-        <v>315.2115326768105</v>
+        <v>6.338943043987854</v>
       </c>
       <c r="E223" t="n">
-        <v>6.0</v>
+        <v>8.062257766723633</v>
       </c>
       <c r="F223" t="n">
         <v>1.0</v>
@@ -20419,19 +20619,19 @@
     </row>
     <row r="224">
       <c r="A224" t="n">
-        <v>18.0</v>
+        <v>11.0</v>
       </c>
       <c r="B224" t="n">
-        <v>41.0</v>
+        <v>19.0</v>
       </c>
       <c r="C224" t="n">
-        <v>14.764822959899902</v>
+        <v>12.041594505310059</v>
       </c>
       <c r="D224" t="n">
-        <v>336.359591450648</v>
+        <v>323.25993313398806</v>
       </c>
       <c r="E224" t="n">
-        <v>8.062257766723633</v>
+        <v>13.892443656921387</v>
       </c>
       <c r="F224" t="n">
         <v>1.0</v>
@@ -20439,19 +20639,19 @@
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>48.0</v>
+        <v>38.0</v>
       </c>
       <c r="B225" t="n">
-        <v>17.0</v>
+        <v>15.0</v>
       </c>
       <c r="C225" t="n">
         <v>15.81138801574707</v>
       </c>
       <c r="D225" t="n">
-        <v>315.2115326768105</v>
+        <v>216.59028435753538</v>
       </c>
       <c r="E225" t="n">
-        <v>23.409399032592773</v>
+        <v>6.7082037925720215</v>
       </c>
       <c r="F225" t="n">
         <v>1.0</v>
@@ -20459,19 +20659,19 @@
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>23.0</v>
+        <v>37.0</v>
       </c>
       <c r="B226" t="n">
-        <v>16.0</v>
+        <v>9.0</v>
       </c>
       <c r="C226" t="n">
-        <v>22.022714614868164</v>
+        <v>18.11077117919922</v>
       </c>
       <c r="D226" t="n">
-        <v>299.7015117237478</v>
+        <v>251.4270412434094</v>
       </c>
       <c r="E226" t="n">
-        <v>9.219544410705566</v>
+        <v>18.384777069091797</v>
       </c>
       <c r="F226" t="n">
         <v>1.0</v>
@@ -20479,19 +20679,19 @@
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>43.0</v>
+        <v>17.0</v>
       </c>
       <c r="B227" t="n">
-        <v>11.0</v>
+        <v>3.0</v>
       </c>
       <c r="C227" t="n">
-        <v>34.65544509887695</v>
+        <v>17.262676239013672</v>
       </c>
       <c r="D227" t="n">
-        <v>8.319952741629265</v>
+        <v>164.42302223578986</v>
       </c>
       <c r="E227" t="n">
-        <v>13.03840446472168</v>
+        <v>5.099019527435303</v>
       </c>
       <c r="F227" t="n">
         <v>1.0</v>
@@ -20499,19 +20699,19 @@
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>24.0</v>
+        <v>18.0</v>
       </c>
       <c r="B228" t="n">
-        <v>10.0</v>
+        <v>41.0</v>
       </c>
       <c r="C228" t="n">
-        <v>25.05992889404297</v>
+        <v>14.764822959899902</v>
       </c>
       <c r="D228" t="n">
-        <v>171.97940109631875</v>
+        <v>336.359591450648</v>
       </c>
       <c r="E228" t="n">
-        <v>12.369317054748535</v>
+        <v>14.142135620117188</v>
       </c>
       <c r="F228" t="n">
         <v>1.0</v>
@@ -20519,19 +20719,19 @@
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
       </c>
       <c r="B229" t="n">
-        <v>21.0</v>
+        <v>27.0</v>
       </c>
       <c r="C229" t="n">
-        <v>18.11077117919922</v>
+        <v>30.479501724243164</v>
       </c>
       <c r="D229" t="n">
-        <v>346.6473834054614</v>
+        <v>298.9856443268601</v>
       </c>
       <c r="E229" t="n">
-        <v>10.770329475402832</v>
+        <v>17.464248657226562</v>
       </c>
       <c r="F229" t="n">
         <v>1.0</v>
@@ -20539,19 +20739,19 @@
     </row>
     <row r="230">
       <c r="A230" t="n">
-        <v>25.0</v>
+        <v>19.0</v>
       </c>
       <c r="B230" t="n">
-        <v>28.0</v>
+        <v>9.0</v>
       </c>
       <c r="C230" t="n">
-        <v>23.0867919921875</v>
+        <v>31.906112670898438</v>
       </c>
       <c r="D230" t="n">
-        <v>240.25810175410237</v>
+        <v>264.5569058120526</v>
       </c>
       <c r="E230" t="n">
-        <v>6.4031243324279785</v>
+        <v>5.0</v>
       </c>
       <c r="F230" t="n">
         <v>1.0</v>
@@ -20559,19 +20759,19 @@
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>13.0</v>
+        <v>40.0</v>
       </c>
       <c r="B231" t="n">
-        <v>23.0</v>
+        <v>7.0</v>
       </c>
       <c r="C231" t="n">
-        <v>29.154760360717773</v>
+        <v>42.20189666748047</v>
       </c>
       <c r="D231" t="n">
         <v>8.319952741629265</v>
       </c>
       <c r="E231" t="n">
-        <v>13.152946472167969</v>
+        <v>10.630146026611328</v>
       </c>
       <c r="F231" t="n">
         <v>1.0</v>
@@ -20591,23 +20791,23 @@
         <v>303.7008314149076</v>
       </c>
       <c r="E232" t="n">
-        <v>25.495098114013672</v>
+        <v>7.8102498054504395</v>
       </c>
       <c r="F232" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="233">
-      <c r="A233" t="s" s="55">
+      <c r="A233" t="s" s="103">
         <v>27</v>
       </c>
-      <c r="B233" s="59" t="n">
+      <c r="B233" s="107" t="n">
         <f>SUM(B205:B232)</f>
-        <v>417.0</v>
-      </c>
-      <c r="E233" s="59" t="n">
+        <v>397.0</v>
+      </c>
+      <c r="E233" s="107" t="n">
         <f>SUM(E205:E232)</f>
-        <v>355.56019163131714</v>
+        <v>310.29214572906494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started to create algorithm for routing nodes more efficiently inside TR for now
</commit_message>
<xml_diff>
--- a/data/TR/results/PVRP_All_Long_Solutions.xlsx
+++ b/data/TR/results/PVRP_All_Long_Solutions.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="pr10.xlsx" r:id="rId3" sheetId="1"/>
     <sheet name="p11.xlsx" r:id="rId4" sheetId="2"/>
+    <sheet name="p1.xlsx" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5398" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7640" uniqueCount="33">
   <si>
     <t>Filename</t>
   </si>
@@ -104,19 +105,313 @@
   <si>
     <t>edu.sru.thangiah.zeus.tr.TRSolutionHierarchy.Heuristics.Selection.TRChooseByHighestDemand</t>
   </si>
+  <si>
+    <t>p1.xlsx</t>
+  </si>
+  <si>
+    <t>edu.sru.thangiah.zeus.tr.TRSolutionHierarchy.Heuristics.Selection.TRSmallestAngleToDepot</t>
+  </si>
+  <si>
+    <t>edu.sru.thangiah.zeus.tr.TRSolutionHierarchy.Heuristics.Selection.TRSmallestAngleClosestDistanceToDepot</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="22">
+  <fonts count="79">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -264,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
@@ -336,6 +631,196 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -32634,4 +33119,1972 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.890625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="99.99609375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.89453125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.26171875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.5390625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.69921875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="154">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="153">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="153">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="153">
+        <v>6</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="153">
+        <v>7</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1302.54345703125</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="153">
+        <v>8</v>
+      </c>
+      <c r="B6" t="n">
+        <v>937.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="153">
+        <v>9</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12">
+      <c r="A12" t="s" s="151">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C12" t="s" s="151">
+        <v>11</v>
+      </c>
+      <c r="D12" t="n" s="152">
+        <v>30.0</v>
+      </c>
+      <c r="E12" t="s" s="151">
+        <v>12</v>
+      </c>
+      <c r="F12" t="n" s="152">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="151">
+        <v>13</v>
+      </c>
+      <c r="B13" t="n" s="152">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="151">
+        <v>14</v>
+      </c>
+      <c r="B14" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C14" t="s" s="151">
+        <v>15</v>
+      </c>
+      <c r="D14" t="n" s="152">
+        <v>160.0</v>
+      </c>
+      <c r="E14" t="s" s="151">
+        <v>16</v>
+      </c>
+      <c r="F14" t="n" s="155">
+        <v>160.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="151">
+        <v>17</v>
+      </c>
+      <c r="B15" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C15" t="s" s="151">
+        <v>18</v>
+      </c>
+      <c r="D15" t="n" s="152">
+        <v>1.0E9</v>
+      </c>
+      <c r="E15" t="s" s="151">
+        <v>19</v>
+      </c>
+      <c r="F15" t="n" s="155">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16"/>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>28.514418468902136</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>160.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>28.514418468902136</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>28.514418468902136</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="151">
+        <v>27</v>
+      </c>
+      <c r="B21" s="155" t="n">
+        <f>SUM(B18:B20)</f>
+        <v>160.0</v>
+      </c>
+      <c r="E21" s="155" t="n">
+        <f>SUM(E18:E20)</f>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25">
+      <c r="A25" t="s" s="151">
+        <v>10</v>
+      </c>
+      <c r="B25" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C25" t="s" s="151">
+        <v>11</v>
+      </c>
+      <c r="D25" t="n" s="152">
+        <v>30.0</v>
+      </c>
+      <c r="E25" t="s" s="151">
+        <v>12</v>
+      </c>
+      <c r="F25" t="n" s="152">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="151">
+        <v>13</v>
+      </c>
+      <c r="B26" t="n" s="152">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="151">
+        <v>14</v>
+      </c>
+      <c r="B27" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C27" t="s" s="151">
+        <v>15</v>
+      </c>
+      <c r="D27" t="n" s="152">
+        <v>160.0</v>
+      </c>
+      <c r="E27" t="s" s="151">
+        <v>16</v>
+      </c>
+      <c r="F27" t="n" s="156">
+        <v>274.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="151">
+        <v>17</v>
+      </c>
+      <c r="B28" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C28" t="s" s="151">
+        <v>18</v>
+      </c>
+      <c r="D28" t="n" s="152">
+        <v>1.0E9</v>
+      </c>
+      <c r="E28" t="s" s="151">
+        <v>19</v>
+      </c>
+      <c r="F28" t="n" s="155">
+        <v>434.6172790527344</v>
+      </c>
+    </row>
+    <row r="29"/>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>28.514418468902136</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B32" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>13.892443656921387</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.26389867071003437</v>
+      </c>
+      <c r="E32" t="n">
+        <v>13.892443656921387</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B33" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>12.041594505310059</v>
+      </c>
+      <c r="D33" t="n">
+        <v>91.66995927244386</v>
+      </c>
+      <c r="E33" t="n">
+        <v>12.083045959472656</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B34" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>8.062257766723633</v>
+      </c>
+      <c r="D34" t="n">
+        <v>108.78051665296746</v>
+      </c>
+      <c r="E34" t="n">
+        <v>14.21267032623291</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="B35" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>25.05992889404297</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.26389867071003437</v>
+      </c>
+      <c r="E35" t="n">
+        <v>30.479501724243164</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B36" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>26.419689178466797</v>
+      </c>
+      <c r="D36" t="n">
+        <v>89.2513328193786</v>
+      </c>
+      <c r="E36" t="n">
+        <v>14.21267032623291</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="B37" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>28.160255432128906</v>
+      </c>
+      <c r="D37" t="n">
+        <v>25.230099921859278</v>
+      </c>
+      <c r="E37" t="n">
+        <v>11.180339813232422</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B38" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>29.154760360717773</v>
+      </c>
+      <c r="D38" t="n">
+        <v>74.84805231058931</v>
+      </c>
+      <c r="E38" t="n">
+        <v>48.30113983154297</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B39" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>31.906112670898438</v>
+      </c>
+      <c r="D39" t="n">
+        <v>101.77727059429026</v>
+      </c>
+      <c r="E39" t="n">
+        <v>14.422204971313477</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B40" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>22.022714614868164</v>
+      </c>
+      <c r="D40" t="n">
+        <v>102.60578990165823</v>
+      </c>
+      <c r="E40" t="n">
+        <v>44.10215377807617</v>
+      </c>
+      <c r="F40" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="B41" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>31.320919036865234</v>
+      </c>
+      <c r="D41" t="n">
+        <v>118.86322454180913</v>
+      </c>
+      <c r="E41" t="n">
+        <v>47.26520919799805</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B42" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>14.142135620117188</v>
+      </c>
+      <c r="D42" t="n">
+        <v>360.0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>27.58622932434082</v>
+      </c>
+      <c r="F42" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B43" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>17.262676239013672</v>
+      </c>
+      <c r="D43" t="n">
+        <v>146.42695159921817</v>
+      </c>
+      <c r="E43" t="n">
+        <v>14.764822959899902</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B44" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>14.764822959899902</v>
+      </c>
+      <c r="D44" t="n">
+        <v>359.35807390192</v>
+      </c>
+      <c r="E44" t="n">
+        <v>14.142135620117188</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="B45" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>118.86322454180913</v>
+      </c>
+      <c r="E45" t="n">
+        <v>37.013511657714844</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="B46" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>30.479501724243164</v>
+      </c>
+      <c r="D46" t="n">
+        <v>163.685684486967</v>
+      </c>
+      <c r="E46" t="n">
+        <v>36.67424011230469</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="B47" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>42.20189666748047</v>
+      </c>
+      <c r="D47" t="n">
+        <v>67.54800976007601</v>
+      </c>
+      <c r="E47" t="n">
+        <v>12.083045959472656</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>28.514418468902136</v>
+      </c>
+      <c r="E48" t="n">
+        <v>42.20189666748047</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="151">
+        <v>27</v>
+      </c>
+      <c r="B49" s="155" t="n">
+        <f>SUM(B31:B48)</f>
+        <v>274.0</v>
+      </c>
+      <c r="E49" s="155" t="n">
+        <f>SUM(E31:E48)</f>
+        <v>434.6172618865967</v>
+      </c>
+    </row>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53">
+      <c r="A53" t="s" s="151">
+        <v>10</v>
+      </c>
+      <c r="B53" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C53" t="s" s="151">
+        <v>11</v>
+      </c>
+      <c r="D53" t="n" s="152">
+        <v>30.0</v>
+      </c>
+      <c r="E53" t="s" s="151">
+        <v>12</v>
+      </c>
+      <c r="F53" t="n" s="152">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="151">
+        <v>13</v>
+      </c>
+      <c r="B54" t="n" s="152">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="151">
+        <v>14</v>
+      </c>
+      <c r="B55" t="n" s="152">
+        <v>1.0</v>
+      </c>
+      <c r="C55" t="s" s="151">
+        <v>15</v>
+      </c>
+      <c r="D55" t="n" s="152">
+        <v>160.0</v>
+      </c>
+      <c r="E55" t="s" s="151">
+        <v>16</v>
+      </c>
+      <c r="F55" t="n" s="155">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="151">
+        <v>17</v>
+      </c>
+      <c r="B56" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C56" t="s" s="151">
+        <v>18</v>
+      </c>
+      <c r="D56" t="n" s="152">
+        <v>1.0E9</v>
+      </c>
+      <c r="E56" t="s" s="151">
+        <v>19</v>
+      </c>
+      <c r="F56" t="n" s="155">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="57"/>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>28.514418468902136</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>28.514418468902136</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="151">
+        <v>27</v>
+      </c>
+      <c r="B61" s="155" t="n">
+        <f>SUM(B59:B60)</f>
+        <v>0.0</v>
+      </c>
+      <c r="E61" s="155" t="n">
+        <f>SUM(E59:E60)</f>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65">
+      <c r="A65" t="s" s="151">
+        <v>10</v>
+      </c>
+      <c r="B65" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C65" t="s" s="151">
+        <v>11</v>
+      </c>
+      <c r="D65" t="n" s="152">
+        <v>30.0</v>
+      </c>
+      <c r="E65" t="s" s="151">
+        <v>12</v>
+      </c>
+      <c r="F65" t="n" s="152">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="151">
+        <v>13</v>
+      </c>
+      <c r="B66" t="n" s="152">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="151">
+        <v>14</v>
+      </c>
+      <c r="B67" t="n" s="152">
+        <v>1.0</v>
+      </c>
+      <c r="C67" t="s" s="151">
+        <v>15</v>
+      </c>
+      <c r="D67" t="n" s="152">
+        <v>160.0</v>
+      </c>
+      <c r="E67" t="s" s="151">
+        <v>16</v>
+      </c>
+      <c r="F67" t="n" s="156">
+        <v>259.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="151">
+        <v>17</v>
+      </c>
+      <c r="B68" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C68" t="s" s="151">
+        <v>18</v>
+      </c>
+      <c r="D68" t="n" s="152">
+        <v>1.0E9</v>
+      </c>
+      <c r="E68" t="s" s="151">
+        <v>19</v>
+      </c>
+      <c r="F68" t="n" s="155">
+        <v>408.1383056640625</v>
+      </c>
+    </row>
+    <row r="69"/>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70" t="s">
+        <v>22</v>
+      </c>
+      <c r="D70" t="s">
+        <v>23</v>
+      </c>
+      <c r="E70" t="s">
+        <v>24</v>
+      </c>
+      <c r="F70" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D71" t="n">
+        <v>28.514418468902136</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="B72" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C72" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>12.791703969604043</v>
+      </c>
+      <c r="E72" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B73" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="C73" t="n">
+        <v>11.401754379272461</v>
+      </c>
+      <c r="D73" t="n">
+        <v>73.15546307766584</v>
+      </c>
+      <c r="E73" t="n">
+        <v>17.029386520385742</v>
+      </c>
+      <c r="F73" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="B74" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="C74" t="n">
+        <v>9.433980941772461</v>
+      </c>
+      <c r="D74" t="n">
+        <v>108.78051665296746</v>
+      </c>
+      <c r="E74" t="n">
+        <v>15.524174690246582</v>
+      </c>
+      <c r="F74" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B75" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C75" t="n">
+        <v>17.20465087890625</v>
+      </c>
+      <c r="D75" t="n">
+        <v>121.51248989975329</v>
+      </c>
+      <c r="E75" t="n">
+        <v>7.8102498054504395</v>
+      </c>
+      <c r="F75" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="B76" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C76" t="n">
+        <v>18.11077117919922</v>
+      </c>
+      <c r="D76" t="n">
+        <v>81.80995407018457</v>
+      </c>
+      <c r="E76" t="n">
+        <v>12.649110794067383</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="B77" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C77" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>36.38123898929359</v>
+      </c>
+      <c r="E77" t="n">
+        <v>7.280109882354736</v>
+      </c>
+      <c r="F77" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="B78" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="C78" t="n">
+        <v>21.63330841064453</v>
+      </c>
+      <c r="D78" t="n">
+        <v>63.43855589488288</v>
+      </c>
+      <c r="E78" t="n">
+        <v>22.203603744506836</v>
+      </c>
+      <c r="F78" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B79" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C79" t="n">
+        <v>28.319604873657227</v>
+      </c>
+      <c r="D79" t="n">
+        <v>19.942293639399168</v>
+      </c>
+      <c r="E79" t="n">
+        <v>7.6157732009887695</v>
+      </c>
+      <c r="F79" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="B80" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="C80" t="n">
+        <v>23.0867919921875</v>
+      </c>
+      <c r="D80" t="n">
+        <v>95.53606437366477</v>
+      </c>
+      <c r="E80" t="n">
+        <v>47.16990661621094</v>
+      </c>
+      <c r="F80" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="B81" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="C81" t="n">
+        <v>29.832868576049805</v>
+      </c>
+      <c r="D81" t="n">
+        <v>75.70224652826852</v>
+      </c>
+      <c r="E81" t="n">
+        <v>43.13930892944336</v>
+      </c>
+      <c r="F81" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B82" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C82" t="n">
+        <v>20.808652877807617</v>
+      </c>
+      <c r="D82" t="n">
+        <v>102.60578990165823</v>
+      </c>
+      <c r="E82" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="F82" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="B83" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C83" t="n">
+        <v>2.2360680103302</v>
+      </c>
+      <c r="D83" t="n">
+        <v>129.74341894996647</v>
+      </c>
+      <c r="E83" t="n">
+        <v>20.59126091003418</v>
+      </c>
+      <c r="F83" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B84" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C84" t="n">
+        <v>32.557640075683594</v>
+      </c>
+      <c r="D84" t="n">
+        <v>131.99193827768573</v>
+      </c>
+      <c r="E84" t="n">
+        <v>32.015621185302734</v>
+      </c>
+      <c r="F84" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="B85" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="C85" t="n">
+        <v>15.81138801574707</v>
+      </c>
+      <c r="D85" t="n">
+        <v>181.26572425653285</v>
+      </c>
+      <c r="E85" t="n">
+        <v>28.460498809814453</v>
+      </c>
+      <c r="F85" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B86" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="C86" t="n">
+        <v>23.0867919921875</v>
+      </c>
+      <c r="D86" t="n">
+        <v>359.35807390192</v>
+      </c>
+      <c r="E86" t="n">
+        <v>34.828147888183594</v>
+      </c>
+      <c r="F86" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="B87" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C87" t="n">
+        <v>29.120439529418945</v>
+      </c>
+      <c r="D87" t="n">
+        <v>138.1185786524879</v>
+      </c>
+      <c r="E87" t="n">
+        <v>16.155494689941406</v>
+      </c>
+      <c r="F87" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B88" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C88" t="n">
+        <v>32.06243896484375</v>
+      </c>
+      <c r="D88" t="n">
+        <v>155.67877217332457</v>
+      </c>
+      <c r="E88" t="n">
+        <v>7.211102485656738</v>
+      </c>
+      <c r="F88" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="B89" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="C89" t="n">
+        <v>31.78049659729004</v>
+      </c>
+      <c r="D89" t="n">
+        <v>359.35807390192</v>
+      </c>
+      <c r="E89" t="n">
+        <v>9.05538558959961</v>
+      </c>
+      <c r="F89" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="B90" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="C90" t="n">
+        <v>38.28837966918945</v>
+      </c>
+      <c r="D90" t="n">
+        <v>36.38123898929359</v>
+      </c>
+      <c r="E90" t="n">
+        <v>18.11077117919922</v>
+      </c>
+      <c r="F90" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D91" t="n">
+        <v>28.514418468902136</v>
+      </c>
+      <c r="E91" t="n">
+        <v>38.28837966918945</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="151">
+        <v>27</v>
+      </c>
+      <c r="B92" s="155" t="n">
+        <f>SUM(B71:B91)</f>
+        <v>259.0</v>
+      </c>
+      <c r="E92" s="155" t="n">
+        <f>SUM(E71:E91)</f>
+        <v>408.1382865905762</v>
+      </c>
+    </row>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96">
+      <c r="A96" t="s" s="151">
+        <v>10</v>
+      </c>
+      <c r="B96" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C96" t="s" s="151">
+        <v>11</v>
+      </c>
+      <c r="D96" t="n" s="152">
+        <v>30.0</v>
+      </c>
+      <c r="E96" t="s" s="151">
+        <v>12</v>
+      </c>
+      <c r="F96" t="n" s="152">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="151">
+        <v>13</v>
+      </c>
+      <c r="B97" t="n" s="152">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="151">
+        <v>14</v>
+      </c>
+      <c r="B98" t="n" s="152">
+        <v>2.0</v>
+      </c>
+      <c r="C98" t="s" s="151">
+        <v>15</v>
+      </c>
+      <c r="D98" t="n" s="152">
+        <v>160.0</v>
+      </c>
+      <c r="E98" t="s" s="151">
+        <v>16</v>
+      </c>
+      <c r="F98" t="n" s="155">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="151">
+        <v>17</v>
+      </c>
+      <c r="B99" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C99" t="s" s="151">
+        <v>18</v>
+      </c>
+      <c r="D99" t="n" s="152">
+        <v>1.0E9</v>
+      </c>
+      <c r="E99" t="s" s="151">
+        <v>19</v>
+      </c>
+      <c r="F99" t="n" s="155">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="100"/>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>20</v>
+      </c>
+      <c r="B101" t="s">
+        <v>21</v>
+      </c>
+      <c r="C101" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101" t="s">
+        <v>23</v>
+      </c>
+      <c r="E101" t="s">
+        <v>24</v>
+      </c>
+      <c r="F101" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D102" t="n">
+        <v>28.514418468902136</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D103" t="n">
+        <v>28.514418468902136</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="151">
+        <v>27</v>
+      </c>
+      <c r="B104" s="155" t="n">
+        <f>SUM(B102:B103)</f>
+        <v>0.0</v>
+      </c>
+      <c r="E104" s="155" t="n">
+        <f>SUM(E102:E103)</f>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108">
+      <c r="A108" t="s" s="151">
+        <v>10</v>
+      </c>
+      <c r="B108" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C108" t="s" s="151">
+        <v>11</v>
+      </c>
+      <c r="D108" t="n" s="152">
+        <v>30.0</v>
+      </c>
+      <c r="E108" t="s" s="151">
+        <v>12</v>
+      </c>
+      <c r="F108" t="n" s="152">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="151">
+        <v>13</v>
+      </c>
+      <c r="B109" t="n" s="152">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="151">
+        <v>14</v>
+      </c>
+      <c r="B110" t="n" s="152">
+        <v>2.0</v>
+      </c>
+      <c r="C110" t="s" s="151">
+        <v>15</v>
+      </c>
+      <c r="D110" t="n" s="152">
+        <v>160.0</v>
+      </c>
+      <c r="E110" t="s" s="151">
+        <v>16</v>
+      </c>
+      <c r="F110" t="n" s="156">
+        <v>244.0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="151">
+        <v>17</v>
+      </c>
+      <c r="B111" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="C111" t="s" s="151">
+        <v>18</v>
+      </c>
+      <c r="D111" t="n" s="152">
+        <v>1.0E9</v>
+      </c>
+      <c r="E111" t="s" s="151">
+        <v>19</v>
+      </c>
+      <c r="F111" t="n" s="155">
+        <v>459.7879333496094</v>
+      </c>
+    </row>
+    <row r="112"/>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>20</v>
+      </c>
+      <c r="B113" t="s">
+        <v>21</v>
+      </c>
+      <c r="C113" t="s">
+        <v>22</v>
+      </c>
+      <c r="D113" t="s">
+        <v>23</v>
+      </c>
+      <c r="E113" t="s">
+        <v>24</v>
+      </c>
+      <c r="F113" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D114" t="n">
+        <v>28.514418468902136</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B115" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="C115" t="n">
+        <v>21.02379608154297</v>
+      </c>
+      <c r="D115" t="n">
+        <v>17.091337924833</v>
+      </c>
+      <c r="E115" t="n">
+        <v>21.02379608154297</v>
+      </c>
+      <c r="F115" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="B116" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="C116" t="n">
+        <v>15.81138801574707</v>
+      </c>
+      <c r="D116" t="n">
+        <v>110.22832770626519</v>
+      </c>
+      <c r="E116" t="n">
+        <v>14.560219764709473</v>
+      </c>
+      <c r="F116" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B117" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="C117" t="n">
+        <v>22.022714614868164</v>
+      </c>
+      <c r="D117" t="n">
+        <v>40.095415674959895</v>
+      </c>
+      <c r="E117" t="n">
+        <v>30.4138126373291</v>
+      </c>
+      <c r="F117" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="B118" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C118" t="n">
+        <v>26.172504425048828</v>
+      </c>
+      <c r="D118" t="n">
+        <v>46.88178417230375</v>
+      </c>
+      <c r="E118" t="n">
+        <v>35.35533905029297</v>
+      </c>
+      <c r="F118" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B119" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="C119" t="n">
+        <v>22.022714614868164</v>
+      </c>
+      <c r="D119" t="n">
+        <v>91.66995927244386</v>
+      </c>
+      <c r="E119" t="n">
+        <v>5.656854152679443</v>
+      </c>
+      <c r="F119" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B120" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C120" t="n">
+        <v>24.73863410949707</v>
+      </c>
+      <c r="D120" t="n">
+        <v>100.38115253922035</v>
+      </c>
+      <c r="E120" t="n">
+        <v>29.681644439697266</v>
+      </c>
+      <c r="F120" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="B121" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C121" t="n">
+        <v>30.870698928833008</v>
+      </c>
+      <c r="D121" t="n">
+        <v>5.435382804439996</v>
+      </c>
+      <c r="E121" t="n">
+        <v>24.59674835205078</v>
+      </c>
+      <c r="F121" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B122" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="C122" t="n">
+        <v>32.4499626159668</v>
+      </c>
+      <c r="D122" t="n">
+        <v>39.048555484699136</v>
+      </c>
+      <c r="E122" t="n">
+        <v>31.016124725341797</v>
+      </c>
+      <c r="F122" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="B123" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C123" t="n">
+        <v>31.320919036865234</v>
+      </c>
+      <c r="D123" t="n">
+        <v>118.86322454180913</v>
+      </c>
+      <c r="E123" t="n">
+        <v>51.26402282714844</v>
+      </c>
+      <c r="F123" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="B124" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="C124" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="D124" t="n">
+        <v>138.1185786524879</v>
+      </c>
+      <c r="E124" t="n">
+        <v>39.051246643066406</v>
+      </c>
+      <c r="F124" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B125" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="C125" t="n">
+        <v>18.11077117919922</v>
+      </c>
+      <c r="D125" t="n">
+        <v>155.67877217332457</v>
+      </c>
+      <c r="E125" t="n">
+        <v>18.973665237426758</v>
+      </c>
+      <c r="F125" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="B126" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="C126" t="n">
+        <v>29.96664810180664</v>
+      </c>
+      <c r="D126" t="n">
+        <v>147.52499422511914</v>
+      </c>
+      <c r="E126" t="n">
+        <v>39.824615478515625</v>
+      </c>
+      <c r="F126" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="B127" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="C127" t="n">
+        <v>39.408119201660156</v>
+      </c>
+      <c r="D127" t="n">
+        <v>89.2513328193786</v>
+      </c>
+      <c r="E127" t="n">
+        <v>19.416488647460938</v>
+      </c>
+      <c r="F127" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="B128" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C128" t="n">
+        <v>43.931766510009766</v>
+      </c>
+      <c r="D128" t="n">
+        <v>75.70224652826852</v>
+      </c>
+      <c r="E128" t="n">
+        <v>6.082762718200684</v>
+      </c>
+      <c r="F128" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="B129" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="C129" t="n">
+        <v>34.65544509887695</v>
+      </c>
+      <c r="D129" t="n">
+        <v>131.99193827768573</v>
+      </c>
+      <c r="E129" t="n">
+        <v>58.215118408203125</v>
+      </c>
+      <c r="F129" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B130" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C130" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D130" t="n">
+        <v>28.514418468902136</v>
+      </c>
+      <c r="E130" t="n">
+        <v>34.65544509887695</v>
+      </c>
+      <c r="F130" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s" s="151">
+        <v>27</v>
+      </c>
+      <c r="B131" s="155" t="n">
+        <f>SUM(B114:B130)</f>
+        <v>244.0</v>
+      </c>
+      <c r="E131" s="155" t="n">
+        <f>SUM(E114:E130)</f>
+        <v>459.7879042625427</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working on making insertion more robust -- to check all combinations when inserting
</commit_message>
<xml_diff>
--- a/data/TR/results/PVRP_All_Long_Solutions.xlsx
+++ b/data/TR/results/PVRP_All_Long_Solutions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="28">
   <si>
     <t>Filename</t>
   </si>
@@ -103,13 +103,88 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="13">
+  <fonts count="28">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -212,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
@@ -254,6 +329,56 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -266,16 +391,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.890625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="99.99609375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.89453125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.26171875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.5390625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.63671875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.11328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="96.51953125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.2890625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.90625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.7734375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.4921875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="22">
+      <c r="A1" t="s" s="52">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -283,7 +408,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="21">
+      <c r="A2" t="s" s="51">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -291,7 +416,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="21">
+      <c r="A3" t="s" s="51">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -299,7 +424,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="21">
+      <c r="A4" t="s" s="51">
         <v>6</v>
       </c>
       <c r="B4" t="n">
@@ -307,23 +432,23 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="21">
+      <c r="A5" t="s" s="51">
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>729.301025390625</v>
+        <v>8.02871296E8</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="21">
+      <c r="A6" t="s" s="51">
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>1458.0</v>
+        <v>6.84096768E8</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="21">
+      <c r="A7" t="s" s="51">
         <v>9</v>
       </c>
       <c r="B7" t="n">
@@ -335,71 +460,71 @@
     <row r="10"/>
     <row r="11"/>
     <row r="12">
-      <c r="A12" t="s" s="19">
+      <c r="A12" t="s" s="49">
         <v>10</v>
       </c>
-      <c r="B12" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C12" t="s" s="19">
+      <c r="B12" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C12" t="s" s="49">
         <v>11</v>
       </c>
-      <c r="D12" t="n" s="20">
+      <c r="D12" t="n" s="50">
         <v>35.0</v>
       </c>
-      <c r="E12" t="s" s="19">
+      <c r="E12" t="s" s="49">
         <v>12</v>
       </c>
-      <c r="F12" t="n" s="20">
+      <c r="F12" t="n" s="50">
         <v>35.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="19">
+      <c r="A13" t="s" s="49">
         <v>13</v>
       </c>
-      <c r="B13" t="n" s="20">
+      <c r="B13" t="n" s="50">
         <v>0.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="19">
+      <c r="A14" t="s" s="49">
         <v>14</v>
       </c>
-      <c r="B14" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C14" t="s" s="19">
+      <c r="B14" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C14" t="s" s="49">
         <v>15</v>
       </c>
-      <c r="D14" t="n" s="20">
+      <c r="D14" t="n" s="50">
         <v>200.0</v>
       </c>
-      <c r="E14" t="s" s="19">
+      <c r="E14" t="s" s="49">
         <v>16</v>
       </c>
-      <c r="F14" t="n" s="23">
-        <v>0.0</v>
+      <c r="F14" t="n" s="53">
+        <v>3.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s" s="19">
+      <c r="A15" t="s" s="49">
         <v>17</v>
       </c>
-      <c r="B15" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C15" t="s" s="19">
+      <c r="B15" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C15" t="s" s="49">
         <v>18</v>
       </c>
-      <c r="D15" t="n" s="20">
+      <c r="D15" t="n" s="50">
         <v>1.0E9</v>
       </c>
-      <c r="E15" t="s" s="19">
+      <c r="E15" t="s" s="49">
         <v>19</v>
       </c>
-      <c r="F15" t="n" s="23">
-        <v>0.0</v>
+      <c r="F15" t="n" s="53">
+        <v>64.49806213378906</v>
       </c>
     </row>
     <row r="16"/>
@@ -464,14 +589,14 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s" s="19">
+      <c r="A20" t="s" s="49">
         <v>27</v>
       </c>
-      <c r="B20" s="23" t="n">
+      <c r="B20" s="54" t="n">
         <f>SUM(B18:B19)</f>
         <v>0.0</v>
       </c>
-      <c r="E20" s="23" t="n">
+      <c r="E20" s="54" t="n">
         <f>SUM(E18:E19)</f>
         <v>0.0</v>
       </c>
@@ -480,71 +605,71 @@
     <row r="22"/>
     <row r="23"/>
     <row r="24">
-      <c r="A24" t="s" s="19">
+      <c r="A24" t="s" s="49">
         <v>10</v>
       </c>
-      <c r="B24" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C24" t="s" s="19">
+      <c r="B24" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C24" t="s" s="49">
         <v>11</v>
       </c>
-      <c r="D24" t="n" s="20">
+      <c r="D24" t="n" s="50">
         <v>35.0</v>
       </c>
-      <c r="E24" t="s" s="19">
+      <c r="E24" t="s" s="49">
         <v>12</v>
       </c>
-      <c r="F24" t="n" s="20">
+      <c r="F24" t="n" s="50">
         <v>35.0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s" s="19">
+      <c r="A25" t="s" s="49">
         <v>13</v>
       </c>
-      <c r="B25" t="n" s="20">
+      <c r="B25" t="n" s="50">
         <v>1.0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s" s="19">
+      <c r="A26" t="s" s="49">
         <v>14</v>
       </c>
-      <c r="B26" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C26" t="s" s="19">
+      <c r="B26" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C26" t="s" s="49">
         <v>15</v>
       </c>
-      <c r="D26" t="n" s="20">
+      <c r="D26" t="n" s="50">
         <v>200.0</v>
       </c>
-      <c r="E26" t="s" s="19">
+      <c r="E26" t="s" s="49">
         <v>16</v>
       </c>
-      <c r="F26" t="n" s="23">
-        <v>0.0</v>
+      <c r="F26" t="n" s="53">
+        <v>3.0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s" s="19">
+      <c r="A27" t="s" s="49">
         <v>17</v>
       </c>
-      <c r="B27" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C27" t="s" s="19">
+      <c r="B27" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C27" t="s" s="49">
         <v>18</v>
       </c>
-      <c r="D27" t="n" s="20">
+      <c r="D27" t="n" s="50">
         <v>1.0E9</v>
       </c>
-      <c r="E27" t="s" s="19">
+      <c r="E27" t="s" s="49">
         <v>19</v>
       </c>
-      <c r="F27" t="n" s="23">
-        <v>0.0</v>
+      <c r="F27" t="n" s="53">
+        <v>64.49806213378906</v>
       </c>
     </row>
     <row r="28"/>
@@ -609,14 +734,14 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s" s="19">
+      <c r="A32" t="s" s="49">
         <v>27</v>
       </c>
-      <c r="B32" s="23" t="n">
+      <c r="B32" s="54" t="n">
         <f>SUM(B30:B31)</f>
         <v>0.0</v>
       </c>
-      <c r="E32" s="23" t="n">
+      <c r="E32" s="54" t="n">
         <f>SUM(E30:E31)</f>
         <v>0.0</v>
       </c>
@@ -625,71 +750,71 @@
     <row r="34"/>
     <row r="35"/>
     <row r="36">
-      <c r="A36" t="s" s="19">
+      <c r="A36" t="s" s="49">
         <v>10</v>
       </c>
-      <c r="B36" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C36" t="s" s="19">
+      <c r="B36" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C36" t="s" s="49">
         <v>11</v>
       </c>
-      <c r="D36" t="n" s="20">
+      <c r="D36" t="n" s="50">
         <v>35.0</v>
       </c>
-      <c r="E36" t="s" s="19">
+      <c r="E36" t="s" s="49">
         <v>12</v>
       </c>
-      <c r="F36" t="n" s="20">
+      <c r="F36" t="n" s="50">
         <v>35.0</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s" s="19">
+      <c r="A37" t="s" s="49">
         <v>13</v>
       </c>
-      <c r="B37" t="n" s="20">
+      <c r="B37" t="n" s="50">
         <v>2.0</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s" s="19">
+      <c r="A38" t="s" s="49">
         <v>14</v>
       </c>
-      <c r="B38" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C38" t="s" s="19">
+      <c r="B38" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C38" t="s" s="49">
         <v>15</v>
       </c>
-      <c r="D38" t="n" s="20">
+      <c r="D38" t="n" s="50">
         <v>200.0</v>
       </c>
-      <c r="E38" t="s" s="19">
+      <c r="E38" t="s" s="49">
         <v>16</v>
       </c>
-      <c r="F38" t="n" s="23">
-        <v>0.0</v>
+      <c r="F38" t="n" s="53">
+        <v>3.0</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s" s="19">
+      <c r="A39" t="s" s="49">
         <v>17</v>
       </c>
-      <c r="B39" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C39" t="s" s="19">
+      <c r="B39" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C39" t="s" s="49">
         <v>18</v>
       </c>
-      <c r="D39" t="n" s="20">
+      <c r="D39" t="n" s="50">
         <v>1.0E9</v>
       </c>
-      <c r="E39" t="s" s="19">
+      <c r="E39" t="s" s="49">
         <v>19</v>
       </c>
-      <c r="F39" t="n" s="23">
-        <v>0.0</v>
+      <c r="F39" t="n" s="53">
+        <v>64.49806213378906</v>
       </c>
     </row>
     <row r="40"/>
@@ -754,14 +879,14 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s" s="19">
+      <c r="A44" t="s" s="49">
         <v>27</v>
       </c>
-      <c r="B44" s="23" t="n">
+      <c r="B44" s="54" t="n">
         <f>SUM(B42:B43)</f>
         <v>0.0</v>
       </c>
-      <c r="E44" s="23" t="n">
+      <c r="E44" s="54" t="n">
         <f>SUM(E42:E43)</f>
         <v>0.0</v>
       </c>
@@ -770,71 +895,71 @@
     <row r="46"/>
     <row r="47"/>
     <row r="48">
-      <c r="A48" t="s" s="19">
+      <c r="A48" t="s" s="49">
         <v>10</v>
       </c>
-      <c r="B48" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C48" t="s" s="19">
+      <c r="B48" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C48" t="s" s="49">
         <v>11</v>
       </c>
-      <c r="D48" t="n" s="20">
+      <c r="D48" t="n" s="50">
         <v>35.0</v>
       </c>
-      <c r="E48" t="s" s="19">
+      <c r="E48" t="s" s="49">
         <v>12</v>
       </c>
-      <c r="F48" t="n" s="20">
+      <c r="F48" t="n" s="50">
         <v>35.0</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="s" s="19">
+      <c r="A49" t="s" s="49">
         <v>13</v>
       </c>
-      <c r="B49" t="n" s="20">
+      <c r="B49" t="n" s="50">
         <v>3.0</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s" s="19">
+      <c r="A50" t="s" s="49">
         <v>14</v>
       </c>
-      <c r="B50" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C50" t="s" s="19">
+      <c r="B50" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C50" t="s" s="49">
         <v>15</v>
       </c>
-      <c r="D50" t="n" s="20">
+      <c r="D50" t="n" s="50">
         <v>200.0</v>
       </c>
-      <c r="E50" t="s" s="19">
+      <c r="E50" t="s" s="49">
         <v>16</v>
       </c>
-      <c r="F50" t="n" s="23">
-        <v>0.0</v>
+      <c r="F50" t="n" s="53">
+        <v>3.0</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="s" s="19">
+      <c r="A51" t="s" s="49">
         <v>17</v>
       </c>
-      <c r="B51" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C51" t="s" s="19">
+      <c r="B51" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C51" t="s" s="49">
         <v>18</v>
       </c>
-      <c r="D51" t="n" s="20">
+      <c r="D51" t="n" s="50">
         <v>1.0E9</v>
       </c>
-      <c r="E51" t="s" s="19">
+      <c r="E51" t="s" s="49">
         <v>19</v>
       </c>
-      <c r="F51" t="n" s="23">
-        <v>0.0</v>
+      <c r="F51" t="n" s="53">
+        <v>64.49806213378906</v>
       </c>
     </row>
     <row r="52"/>
@@ -899,14 +1024,14 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="s" s="19">
+      <c r="A56" t="s" s="49">
         <v>27</v>
       </c>
-      <c r="B56" s="23" t="n">
+      <c r="B56" s="54" t="n">
         <f>SUM(B54:B55)</f>
         <v>0.0</v>
       </c>
-      <c r="E56" s="23" t="n">
+      <c r="E56" s="54" t="n">
         <f>SUM(E54:E55)</f>
         <v>0.0</v>
       </c>
@@ -915,71 +1040,71 @@
     <row r="58"/>
     <row r="59"/>
     <row r="60">
-      <c r="A60" t="s" s="19">
+      <c r="A60" t="s" s="49">
         <v>10</v>
       </c>
-      <c r="B60" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C60" t="s" s="19">
+      <c r="B60" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C60" t="s" s="49">
         <v>11</v>
       </c>
-      <c r="D60" t="n" s="20">
+      <c r="D60" t="n" s="50">
         <v>35.0</v>
       </c>
-      <c r="E60" t="s" s="19">
+      <c r="E60" t="s" s="49">
         <v>12</v>
       </c>
-      <c r="F60" t="n" s="20">
+      <c r="F60" t="n" s="50">
         <v>35.0</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="s" s="19">
+      <c r="A61" t="s" s="49">
         <v>13</v>
       </c>
-      <c r="B61" t="n" s="20">
+      <c r="B61" t="n" s="50">
         <v>4.0</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="s" s="19">
+      <c r="A62" t="s" s="49">
         <v>14</v>
       </c>
-      <c r="B62" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C62" t="s" s="19">
+      <c r="B62" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C62" t="s" s="49">
         <v>15</v>
       </c>
-      <c r="D62" t="n" s="20">
+      <c r="D62" t="n" s="50">
         <v>200.0</v>
       </c>
-      <c r="E62" t="s" s="19">
+      <c r="E62" t="s" s="49">
         <v>16</v>
       </c>
-      <c r="F62" t="n" s="23">
-        <v>0.0</v>
+      <c r="F62" t="n" s="53">
+        <v>3.0</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="s" s="19">
+      <c r="A63" t="s" s="49">
         <v>17</v>
       </c>
-      <c r="B63" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C63" t="s" s="19">
+      <c r="B63" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C63" t="s" s="49">
         <v>18</v>
       </c>
-      <c r="D63" t="n" s="20">
+      <c r="D63" t="n" s="50">
         <v>1.0E9</v>
       </c>
-      <c r="E63" t="s" s="19">
+      <c r="E63" t="s" s="49">
         <v>19</v>
       </c>
-      <c r="F63" t="n" s="23">
-        <v>0.0</v>
+      <c r="F63" t="n" s="53">
+        <v>64.49806213378906</v>
       </c>
     </row>
     <row r="64"/>
@@ -1044,14 +1169,14 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="s" s="19">
+      <c r="A68" t="s" s="49">
         <v>27</v>
       </c>
-      <c r="B68" s="23" t="n">
+      <c r="B68" s="54" t="n">
         <f>SUM(B66:B67)</f>
         <v>0.0</v>
       </c>
-      <c r="E68" s="23" t="n">
+      <c r="E68" s="54" t="n">
         <f>SUM(E66:E67)</f>
         <v>0.0</v>
       </c>
@@ -1060,71 +1185,71 @@
     <row r="70"/>
     <row r="71"/>
     <row r="72">
-      <c r="A72" t="s" s="19">
+      <c r="A72" t="s" s="49">
         <v>10</v>
       </c>
-      <c r="B72" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C72" t="s" s="19">
+      <c r="B72" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C72" t="s" s="49">
         <v>11</v>
       </c>
-      <c r="D72" t="n" s="20">
+      <c r="D72" t="n" s="50">
         <v>35.0</v>
       </c>
-      <c r="E72" t="s" s="19">
+      <c r="E72" t="s" s="49">
         <v>12</v>
       </c>
-      <c r="F72" t="n" s="20">
+      <c r="F72" t="n" s="50">
         <v>35.0</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="s" s="19">
+      <c r="A73" t="s" s="49">
         <v>13</v>
       </c>
-      <c r="B73" t="n" s="20">
+      <c r="B73" t="n" s="50">
         <v>5.0</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="s" s="19">
+      <c r="A74" t="s" s="49">
         <v>14</v>
       </c>
-      <c r="B74" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C74" t="s" s="19">
+      <c r="B74" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C74" t="s" s="49">
         <v>15</v>
       </c>
-      <c r="D74" t="n" s="20">
+      <c r="D74" t="n" s="50">
         <v>200.0</v>
       </c>
-      <c r="E74" t="s" s="19">
+      <c r="E74" t="s" s="49">
         <v>16</v>
       </c>
-      <c r="F74" t="n" s="23">
-        <v>0.0</v>
+      <c r="F74" t="n" s="53">
+        <v>3.0</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="s" s="19">
+      <c r="A75" t="s" s="49">
         <v>17</v>
       </c>
-      <c r="B75" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C75" t="s" s="19">
+      <c r="B75" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C75" t="s" s="49">
         <v>18</v>
       </c>
-      <c r="D75" t="n" s="20">
+      <c r="D75" t="n" s="50">
         <v>1.0E9</v>
       </c>
-      <c r="E75" t="s" s="19">
+      <c r="E75" t="s" s="49">
         <v>19</v>
       </c>
-      <c r="F75" t="n" s="23">
-        <v>0.0</v>
+      <c r="F75" t="n" s="53">
+        <v>64.49806213378906</v>
       </c>
     </row>
     <row r="76"/>
@@ -1189,14 +1314,14 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="s" s="19">
+      <c r="A80" t="s" s="49">
         <v>27</v>
       </c>
-      <c r="B80" s="23" t="n">
+      <c r="B80" s="54" t="n">
         <f>SUM(B78:B79)</f>
         <v>0.0</v>
       </c>
-      <c r="E80" s="23" t="n">
+      <c r="E80" s="54" t="n">
         <f>SUM(E78:E79)</f>
         <v>0.0</v>
       </c>
@@ -1205,71 +1330,71 @@
     <row r="82"/>
     <row r="83"/>
     <row r="84">
-      <c r="A84" t="s" s="19">
+      <c r="A84" t="s" s="49">
         <v>10</v>
       </c>
-      <c r="B84" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C84" t="s" s="19">
+      <c r="B84" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C84" t="s" s="49">
         <v>11</v>
       </c>
-      <c r="D84" t="n" s="20">
+      <c r="D84" t="n" s="50">
         <v>35.0</v>
       </c>
-      <c r="E84" t="s" s="19">
+      <c r="E84" t="s" s="49">
         <v>12</v>
       </c>
-      <c r="F84" t="n" s="20">
+      <c r="F84" t="n" s="50">
         <v>35.0</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="s" s="19">
+      <c r="A85" t="s" s="49">
         <v>13</v>
       </c>
-      <c r="B85" t="n" s="20">
+      <c r="B85" t="n" s="50">
         <v>6.0</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="s" s="19">
+      <c r="A86" t="s" s="49">
         <v>14</v>
       </c>
-      <c r="B86" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C86" t="s" s="19">
+      <c r="B86" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C86" t="s" s="49">
         <v>15</v>
       </c>
-      <c r="D86" t="n" s="20">
+      <c r="D86" t="n" s="50">
         <v>200.0</v>
       </c>
-      <c r="E86" t="s" s="19">
+      <c r="E86" t="s" s="49">
         <v>16</v>
       </c>
-      <c r="F86" t="n" s="23">
-        <v>0.0</v>
+      <c r="F86" t="n" s="53">
+        <v>3.0</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="s" s="19">
+      <c r="A87" t="s" s="49">
         <v>17</v>
       </c>
-      <c r="B87" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C87" t="s" s="19">
+      <c r="B87" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C87" t="s" s="49">
         <v>18</v>
       </c>
-      <c r="D87" t="n" s="20">
+      <c r="D87" t="n" s="50">
         <v>1.0E9</v>
       </c>
-      <c r="E87" t="s" s="19">
+      <c r="E87" t="s" s="49">
         <v>19</v>
       </c>
-      <c r="F87" t="n" s="23">
-        <v>0.0</v>
+      <c r="F87" t="n" s="53">
+        <v>64.49806213378906</v>
       </c>
     </row>
     <row r="88"/>
@@ -1334,14 +1459,14 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="s" s="19">
+      <c r="A92" t="s" s="49">
         <v>27</v>
       </c>
-      <c r="B92" s="23" t="n">
+      <c r="B92" s="54" t="n">
         <f>SUM(B90:B91)</f>
         <v>0.0</v>
       </c>
-      <c r="E92" s="23" t="n">
+      <c r="E92" s="54" t="n">
         <f>SUM(E90:E91)</f>
         <v>0.0</v>
       </c>
@@ -1350,70 +1475,70 @@
     <row r="94"/>
     <row r="95"/>
     <row r="96">
-      <c r="A96" t="s" s="19">
+      <c r="A96" t="s" s="49">
         <v>10</v>
       </c>
-      <c r="B96" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C96" t="s" s="19">
+      <c r="B96" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C96" t="s" s="49">
         <v>11</v>
       </c>
-      <c r="D96" t="n" s="20">
+      <c r="D96" t="n" s="50">
         <v>35.0</v>
       </c>
-      <c r="E96" t="s" s="19">
+      <c r="E96" t="s" s="49">
         <v>12</v>
       </c>
-      <c r="F96" t="n" s="20">
+      <c r="F96" t="n" s="50">
         <v>35.0</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="s" s="19">
+      <c r="A97" t="s" s="49">
         <v>13</v>
       </c>
-      <c r="B97" t="n" s="20">
+      <c r="B97" t="n" s="50">
         <v>7.0</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="s" s="19">
+      <c r="A98" t="s" s="49">
         <v>14</v>
       </c>
-      <c r="B98" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C98" t="s" s="19">
+      <c r="B98" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C98" t="s" s="49">
         <v>15</v>
       </c>
-      <c r="D98" t="n" s="20">
+      <c r="D98" t="n" s="50">
         <v>200.0</v>
       </c>
-      <c r="E98" t="s" s="19">
+      <c r="E98" t="s" s="49">
         <v>16</v>
       </c>
-      <c r="F98" t="n" s="24">
+      <c r="F98" t="n" s="54">
         <v>1458.0</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="s" s="19">
+      <c r="A99" t="s" s="49">
         <v>17</v>
       </c>
-      <c r="B99" t="n" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="C99" t="s" s="19">
+      <c r="B99" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="C99" t="s" s="49">
         <v>18</v>
       </c>
-      <c r="D99" t="n" s="20">
+      <c r="D99" t="n" s="50">
         <v>1.0E9</v>
       </c>
-      <c r="E99" t="s" s="19">
+      <c r="E99" t="s" s="49">
         <v>19</v>
       </c>
-      <c r="F99" t="n" s="23">
+      <c r="F99" t="n" s="53">
         <v>729.301025390625</v>
       </c>
     </row>
@@ -3479,14 +3604,14 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" t="s" s="19">
+      <c r="A204" t="s" s="49">
         <v>27</v>
       </c>
-      <c r="B204" s="23" t="n">
+      <c r="B204" s="53" t="n">
         <f>SUM(B102:B203)</f>
         <v>1458.0</v>
       </c>
-      <c r="E204" s="23" t="n">
+      <c r="E204" s="53" t="n">
         <f>SUM(E102:E203)</f>
         <v>729.3009746074677</v>
       </c>

</xml_diff>